<commit_message>
Add RTs for all trial types
</commit_message>
<xml_diff>
--- a/code/total_df_n46.xlsx
+++ b/code/total_df_n46.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-mid-clean/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB1AB5D-EBCA-B749-845E-937ED71418CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47427523-8FDB-9F43-97DD-7BB05900516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="199">
   <si>
     <t>Sub</t>
   </si>
@@ -606,6 +606,33 @@
   </si>
   <si>
     <t>zstat_DMN_VS_LG_minus_LL</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>SG-N</t>
+  </si>
+  <si>
+    <t>SL_N</t>
+  </si>
+  <si>
+    <t>LG-SG</t>
+  </si>
+  <si>
+    <t>LL_SL</t>
   </si>
 </sst>
 </file>
@@ -1026,13 +1053,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CT47"/>
+  <dimension ref="A1:DG47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CP14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CL1" sqref="CL1:CL1048576"/>
+      <selection pane="bottomRight" activeCell="DH26" sqref="DH26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1047,7 +1074,7 @@
     <col min="94" max="96" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="42" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:111" ht="42" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1342,8 +1369,47 @@
       <c r="CT1" s="9" t="s">
         <v>183</v>
       </c>
+      <c r="CU1" t="s">
+        <v>190</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>191</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>192</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>193</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>194</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>1</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>2</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>195</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>3</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>196</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>4</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="2" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -1656,8 +1722,47 @@
       <c r="CT2" s="2">
         <v>-0.85166682329999999</v>
       </c>
+      <c r="CU2">
+        <v>0.305434638867154</v>
+      </c>
+      <c r="CV2">
+        <v>0.32050712750060401</v>
+      </c>
+      <c r="CW2">
+        <v>0.332187023188453</v>
+      </c>
+      <c r="CX2">
+        <v>0.362249740224797</v>
+      </c>
+      <c r="CY2">
+        <v>0.30837125348625699</v>
+      </c>
+      <c r="CZ2">
+        <v>-8.5370806711060794E-3</v>
+      </c>
+      <c r="DA2">
+        <v>-2.6752384321298402E-2</v>
+      </c>
+      <c r="DB2">
+        <v>-1.16798956878483E-2</v>
+      </c>
+      <c r="DC2">
+        <v>-2.38157697021961E-2</v>
+      </c>
+      <c r="DD2">
+        <v>3.0062717036344101E-2</v>
+      </c>
+      <c r="DE2">
+        <v>-2.9366146191023199E-3</v>
+      </c>
+      <c r="DF2">
+        <v>-1.50724886334501E-2</v>
+      </c>
+      <c r="DG2">
+        <v>-5.3878486738540197E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1970,8 +2075,47 @@
       <c r="CT3" s="2">
         <v>0.1026903936</v>
       </c>
+      <c r="CU3">
+        <v>0.37713703014014699</v>
+      </c>
+      <c r="CV3">
+        <v>0.34409770040656401</v>
+      </c>
+      <c r="CW3">
+        <v>0.32311334281985099</v>
+      </c>
+      <c r="CX3">
+        <v>0.389765408923267</v>
+      </c>
+      <c r="CY3">
+        <v>0.30858965820516399</v>
+      </c>
+      <c r="CZ3">
+        <v>-6.1688701992225795E-4</v>
+      </c>
+      <c r="DA3">
+        <v>5.40236873202957E-2</v>
+      </c>
+      <c r="DB3">
+        <v>2.09843575867125E-2</v>
+      </c>
+      <c r="DC3">
+        <v>-1.4523684614687201E-2</v>
+      </c>
+      <c r="DD3">
+        <v>6.6652066103415494E-2</v>
+      </c>
+      <c r="DE3">
+        <v>6.8547371934982906E-2</v>
+      </c>
+      <c r="DF3">
+        <v>3.3039329733583103E-2</v>
+      </c>
+      <c r="DG3">
+        <v>-8.1175750718102693E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -2284,8 +2428,47 @@
       <c r="CT4" s="2">
         <v>0.54129364430000004</v>
       </c>
+      <c r="CU4">
+        <v>0.34347991854883703</v>
+      </c>
+      <c r="CV4">
+        <v>0.33897643524687698</v>
+      </c>
+      <c r="CW4">
+        <v>0.32272362557705397</v>
+      </c>
+      <c r="CX4">
+        <v>0.34278606483712698</v>
+      </c>
+      <c r="CY4">
+        <v>0.302930305479094</v>
+      </c>
+      <c r="CZ4">
+        <v>-2.4563787987322799E-3</v>
+      </c>
+      <c r="DA4">
+        <v>2.07562929717823E-2</v>
+      </c>
+      <c r="DB4">
+        <v>1.6252809669822399E-2</v>
+      </c>
+      <c r="DC4">
+        <v>-1.97933200979605E-2</v>
+      </c>
+      <c r="DD4">
+        <v>2.0062439260072999E-2</v>
+      </c>
+      <c r="DE4">
+        <v>4.0549613069742897E-2</v>
+      </c>
+      <c r="DF4">
+        <v>4.5034833019599301E-3</v>
+      </c>
+      <c r="DG4">
+        <v>-3.9855759358033503E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
@@ -2598,8 +2781,47 @@
       <c r="CT5" s="2">
         <v>0.65709044309999998</v>
       </c>
+      <c r="CU5">
+        <v>0.271466309786774</v>
+      </c>
+      <c r="CV5">
+        <v>0.27853118465282001</v>
+      </c>
+      <c r="CW5">
+        <v>0.294866868120152</v>
+      </c>
+      <c r="CX5">
+        <v>0.29255829763133001</v>
+      </c>
+      <c r="CY5">
+        <v>0.271871120959986</v>
+      </c>
+      <c r="CZ5">
+        <v>-5.2963112164953899E-3</v>
+      </c>
+      <c r="DA5">
+        <v>-2.3400558333378198E-2</v>
+      </c>
+      <c r="DB5">
+        <v>-1.6335683467332201E-2</v>
+      </c>
+      <c r="DC5">
+        <v>-2.2995747160166499E-2</v>
+      </c>
+      <c r="DD5">
+        <v>-2.3085704888217099E-3</v>
+      </c>
+      <c r="DE5">
+        <v>-4.0481117321178301E-4</v>
+      </c>
+      <c r="DF5">
+        <v>-7.0648748660460097E-3</v>
+      </c>
+      <c r="DG5">
+        <v>-2.06871766713447E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -2912,8 +3134,47 @@
       <c r="CT6" s="2">
         <v>-0.74139154389999995</v>
       </c>
+      <c r="CU6">
+        <v>0.27033338195178602</v>
+      </c>
+      <c r="CV6">
+        <v>0.27706846105866101</v>
+      </c>
+      <c r="CW6">
+        <v>0.28496288182213902</v>
+      </c>
+      <c r="CX6">
+        <v>0.27218974754214198</v>
+      </c>
+      <c r="CY6">
+        <v>0.277509949752129</v>
+      </c>
+      <c r="CZ6">
+        <v>-1.6783792026607001E-3</v>
+      </c>
+      <c r="DA6">
+        <v>-1.46294998703524E-2</v>
+      </c>
+      <c r="DB6">
+        <v>-7.8944207634776796E-3</v>
+      </c>
+      <c r="DC6">
+        <v>-7.4529320700094104E-3</v>
+      </c>
+      <c r="DD6">
+        <v>-1.2773134279996099E-2</v>
+      </c>
+      <c r="DE6">
+        <v>-7.1765678003430297E-3</v>
+      </c>
+      <c r="DF6">
+        <v>-6.7350791068747596E-3</v>
+      </c>
+      <c r="DG6">
+        <v>5.3202022099867402E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3226,8 +3487,47 @@
       <c r="CT7" s="2">
         <v>-0.35477407439999997</v>
       </c>
+      <c r="CU7">
+        <v>0.28031748597277301</v>
+      </c>
+      <c r="CV7">
+        <v>0.31086552736814999</v>
+      </c>
+      <c r="CW7">
+        <v>0.295282690494786</v>
+      </c>
+      <c r="CX7">
+        <v>0.318008447065949</v>
+      </c>
+      <c r="CY7">
+        <v>0.29928748914971898</v>
+      </c>
+      <c r="CZ7">
+        <v>-4.3021003699063101E-3</v>
+      </c>
+      <c r="DA7">
+        <v>-1.49652045220136E-2</v>
+      </c>
+      <c r="DB7">
+        <v>1.55828368733637E-2</v>
+      </c>
+      <c r="DC7">
+        <v>4.0047986549325201E-3</v>
+      </c>
+      <c r="DD7">
+        <v>2.2725756571162398E-2</v>
+      </c>
+      <c r="DE7">
+        <v>-1.8970003176946099E-2</v>
+      </c>
+      <c r="DF7">
+        <v>-3.0548041395377298E-2</v>
+      </c>
+      <c r="DG7">
+        <v>-1.8720957916229901E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -3540,8 +3840,47 @@
       <c r="CT8" s="2">
         <v>-0.39519033980000001</v>
       </c>
+      <c r="CU8">
+        <v>0.260252866370137</v>
+      </c>
+      <c r="CV8">
+        <v>0.29065276565961501</v>
+      </c>
+      <c r="CW8">
+        <v>0.302461104583926</v>
+      </c>
+      <c r="CX8">
+        <v>0.28393655980471499</v>
+      </c>
+      <c r="CY8">
+        <v>0.27895491209346801</v>
+      </c>
+      <c r="CZ8">
+        <v>-7.22114126464084E-3</v>
+      </c>
+      <c r="DA8">
+        <v>-4.2208238213788697E-2</v>
+      </c>
+      <c r="DB8">
+        <v>-1.18083389243111E-2</v>
+      </c>
+      <c r="DC8">
+        <v>-2.3506192490458402E-2</v>
+      </c>
+      <c r="DD8">
+        <v>-1.8524544779211199E-2</v>
+      </c>
+      <c r="DE8">
+        <v>-1.8702045723330198E-2</v>
+      </c>
+      <c r="DF8">
+        <v>-3.0399899289477599E-2</v>
+      </c>
+      <c r="DG8">
+        <v>-4.9816477112471997E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -3854,8 +4193,47 @@
       <c r="CT9" s="2">
         <v>-0.61659799680000005</v>
       </c>
+      <c r="CU9">
+        <v>0.33834768389351599</v>
+      </c>
+      <c r="CV9">
+        <v>0.31042992940638198</v>
+      </c>
+      <c r="CW9">
+        <v>0.36112862802110601</v>
+      </c>
+      <c r="CX9">
+        <v>0.33093400194775302</v>
+      </c>
+      <c r="CY9">
+        <v>0.30117361911106799</v>
+      </c>
+      <c r="CZ9">
+        <v>-6.0413272419412101E-3</v>
+      </c>
+      <c r="DA9">
+        <v>-2.2780944127589398E-2</v>
+      </c>
+      <c r="DB9">
+        <v>-5.0698698614723897E-2</v>
+      </c>
+      <c r="DC9">
+        <v>-5.9955008910037501E-2</v>
+      </c>
+      <c r="DD9">
+        <v>-3.0194626073352899E-2</v>
+      </c>
+      <c r="DE9">
+        <v>3.7174064782448099E-2</v>
+      </c>
+      <c r="DF9">
+        <v>2.7917754487134499E-2</v>
+      </c>
+      <c r="DG9">
+        <v>-2.9760382836684501E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -4168,8 +4546,47 @@
       <c r="CT10" s="2">
         <v>0.19609320699999999</v>
       </c>
+      <c r="CU10">
+        <v>0.270464802962123</v>
+      </c>
+      <c r="CV10">
+        <v>0.27610288557389101</v>
+      </c>
+      <c r="CW10">
+        <v>0.28752696858191401</v>
+      </c>
+      <c r="CX10">
+        <v>0.29879739821717499</v>
+      </c>
+      <c r="CY10">
+        <v>0.26873461768263901</v>
+      </c>
+      <c r="CZ10">
+        <v>-5.1110985475263798E-3</v>
+      </c>
+      <c r="DA10">
+        <v>-1.70621656197909E-2</v>
+      </c>
+      <c r="DB10">
+        <v>-1.1424083008023399E-2</v>
+      </c>
+      <c r="DC10">
+        <v>-1.8792350899275299E-2</v>
+      </c>
+      <c r="DD10">
+        <v>1.1270429635260299E-2</v>
+      </c>
+      <c r="DE10">
+        <v>1.7301852794844299E-3</v>
+      </c>
+      <c r="DF10">
+        <v>-5.6380826117674501E-3</v>
+      </c>
+      <c r="DG10">
+        <v>-3.0062780534535701E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -4482,8 +4899,47 @@
       <c r="CT11" s="2">
         <v>-0.46680769779999998</v>
       </c>
+      <c r="CU11">
+        <v>0.28478656522929602</v>
+      </c>
+      <c r="CV11">
+        <v>0.322761286923196</v>
+      </c>
+      <c r="CW11">
+        <v>0.29669485258636902</v>
+      </c>
+      <c r="CX11">
+        <v>0.33304927079007002</v>
+      </c>
+      <c r="CY11">
+        <v>0.28506881650537202</v>
+      </c>
+      <c r="CZ11">
+        <v>-7.8206785297620096E-3</v>
+      </c>
+      <c r="DA11">
+        <v>-1.1908287357073199E-2</v>
+      </c>
+      <c r="DB11">
+        <v>2.6066434336826198E-2</v>
+      </c>
+      <c r="DC11">
+        <v>-1.1626036080997401E-2</v>
+      </c>
+      <c r="DD11">
+        <v>3.6354418203700299E-2</v>
+      </c>
+      <c r="DE11">
+        <v>-2.8225127607584E-4</v>
+      </c>
+      <c r="DF11">
+        <v>-3.7974721693899399E-2</v>
+      </c>
+      <c r="DG11">
+        <v>-4.7980454284697702E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -4796,8 +5252,47 @@
       <c r="CT12" s="2">
         <v>-0.22571641079999999</v>
       </c>
+      <c r="CU12">
+        <v>0.24546278372872599</v>
+      </c>
+      <c r="CV12">
+        <v>0.25314377364702501</v>
+      </c>
+      <c r="CW12">
+        <v>0.25403052347246502</v>
+      </c>
+      <c r="CX12">
+        <v>0.25497810076922101</v>
+      </c>
+      <c r="CY12">
+        <v>0.249503193655982</v>
+      </c>
+      <c r="CZ12">
+        <v>-1.8750690422685899E-3</v>
+      </c>
+      <c r="DA12">
+        <v>-8.5677397437393596E-3</v>
+      </c>
+      <c r="DB12">
+        <v>-8.8674982544034698E-4</v>
+      </c>
+      <c r="DC12">
+        <v>-4.5273298164829603E-3</v>
+      </c>
+      <c r="DD12">
+        <v>9.4757729675620697E-4</v>
+      </c>
+      <c r="DE12">
+        <v>-4.0404099272564001E-3</v>
+      </c>
+      <c r="DF12">
+        <v>-7.6809899182990098E-3</v>
+      </c>
+      <c r="DG12">
+        <v>-5.4749071132391596E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -5110,8 +5605,47 @@
       <c r="CT13" s="2">
         <v>0.75431486729999997</v>
       </c>
+      <c r="CU13">
+        <v>0.29833598533878097</v>
+      </c>
+      <c r="CV13">
+        <v>0.34576657786965298</v>
+      </c>
+      <c r="CW13">
+        <v>0.315847488935105</v>
+      </c>
+      <c r="CX13">
+        <v>0.33085254079196602</v>
+      </c>
+      <c r="CY13">
+        <v>0.298982144508045</v>
+      </c>
+      <c r="CZ13">
+        <v>-8.1198454884412793E-3</v>
+      </c>
+      <c r="DA13">
+        <v>-1.7511503596324401E-2</v>
+      </c>
+      <c r="DB13">
+        <v>2.9919088934548199E-2</v>
+      </c>
+      <c r="DC13">
+        <v>-1.6865344427060301E-2</v>
+      </c>
+      <c r="DD13">
+        <v>1.5005051856860499E-2</v>
+      </c>
+      <c r="DE13">
+        <v>-6.4615916926413699E-4</v>
+      </c>
+      <c r="DF13">
+        <v>-4.7430592530872603E-2</v>
+      </c>
+      <c r="DG13">
+        <v>-3.1870396283920799E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -5424,8 +5958,47 @@
       <c r="CT14" s="2">
         <v>0.4275285996</v>
       </c>
+      <c r="CU14">
+        <v>0.55924635590054095</v>
+      </c>
+      <c r="CV14">
+        <v>0.52810588863212604</v>
+      </c>
+      <c r="CW14">
+        <v>0.48599444975843598</v>
+      </c>
+      <c r="CX14">
+        <v>0.57096491596894305</v>
+      </c>
+      <c r="CY14">
+        <v>0.478740440797992</v>
+      </c>
+      <c r="CZ14">
+        <v>3.5099209136602E-4</v>
+      </c>
+      <c r="DA14">
+        <v>7.3251906142104403E-2</v>
+      </c>
+      <c r="DB14">
+        <v>4.2111438873689601E-2</v>
+      </c>
+      <c r="DC14">
+        <v>-7.2540089604444802E-3</v>
+      </c>
+      <c r="DD14">
+        <v>8.4970466210506801E-2</v>
+      </c>
+      <c r="DE14">
+        <v>8.0505915102548897E-2</v>
+      </c>
+      <c r="DF14">
+        <v>3.1140467268414702E-2</v>
+      </c>
+      <c r="DG14">
+        <v>-9.2224475170951295E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -5738,8 +6311,47 @@
       <c r="CT15" s="2">
         <v>-0.2368191976</v>
       </c>
+      <c r="CU15">
+        <v>0.27883449981891301</v>
+      </c>
+      <c r="CV15">
+        <v>0.25725000037527901</v>
+      </c>
+      <c r="CW15">
+        <v>0.29304862715798602</v>
+      </c>
+      <c r="CX15">
+        <v>0.34862338516904801</v>
+      </c>
+      <c r="CY15">
+        <v>0.305491818497102</v>
+      </c>
+      <c r="CZ15">
+        <v>-1.66557165916207E-3</v>
+      </c>
+      <c r="DA15">
+        <v>-1.42141273390734E-2</v>
+      </c>
+      <c r="DB15">
+        <v>-3.5798626782707198E-2</v>
+      </c>
+      <c r="DC15">
+        <v>1.24431913391163E-2</v>
+      </c>
+      <c r="DD15">
+        <v>5.5574758011061903E-2</v>
+      </c>
+      <c r="DE15">
+        <v>-2.6657318678189702E-2</v>
+      </c>
+      <c r="DF15">
+        <v>2.15844994436338E-2</v>
+      </c>
+      <c r="DG15">
+        <v>-4.31315666719456E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -6052,8 +6664,47 @@
       <c r="CT16" s="2">
         <v>0.65512747930000004</v>
       </c>
+      <c r="CU16">
+        <v>0.26968774611941598</v>
+      </c>
+      <c r="CV16">
+        <v>0.29450151343735298</v>
+      </c>
+      <c r="CW16">
+        <v>0.28823237660981199</v>
+      </c>
+      <c r="CX16">
+        <v>0.268033032094535</v>
+      </c>
+      <c r="CY16">
+        <v>0.28180007770151799</v>
+      </c>
+      <c r="CZ16">
+        <v>-2.57311793640319E-3</v>
+      </c>
+      <c r="DA16">
+        <v>-1.8544630490396199E-2</v>
+      </c>
+      <c r="DB16">
+        <v>6.2691368275409297E-3</v>
+      </c>
+      <c r="DC16">
+        <v>-6.4322989082938797E-3</v>
+      </c>
+      <c r="DD16">
+        <v>-2.01993445152766E-2</v>
+      </c>
+      <c r="DE16">
+        <v>-1.2112331582102299E-2</v>
+      </c>
+      <c r="DF16">
+        <v>-2.4813767317937101E-2</v>
+      </c>
+      <c r="DG16">
+        <v>1.3767045606982701E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -6366,8 +7017,47 @@
       <c r="CT17" s="2">
         <v>0.33876507109999998</v>
       </c>
+      <c r="CU17">
+        <v>0.29193674297130201</v>
+      </c>
+      <c r="CV17">
+        <v>0.29208420826762399</v>
+      </c>
+      <c r="CW17">
+        <v>0.32701431243913198</v>
+      </c>
+      <c r="CX17">
+        <v>0.29602516900922599</v>
+      </c>
+      <c r="CY17">
+        <v>0.33810273605922703</v>
+      </c>
+      <c r="CZ17">
+        <v>1.2814968504244299E-3</v>
+      </c>
+      <c r="DA17">
+        <v>-3.5077569467830402E-2</v>
+      </c>
+      <c r="DB17">
+        <v>-3.4930104171507902E-2</v>
+      </c>
+      <c r="DC17">
+        <v>1.10884236200945E-2</v>
+      </c>
+      <c r="DD17">
+        <v>-3.0989143429906101E-2</v>
+      </c>
+      <c r="DE17">
+        <v>-4.6165993087925003E-2</v>
+      </c>
+      <c r="DF17">
+        <v>-1.47465296322479E-4</v>
+      </c>
+      <c r="DG17">
+        <v>4.2077567050000597E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -6680,8 +7370,47 @@
       <c r="CT18" s="2">
         <v>0.26996217700000003</v>
       </c>
+      <c r="CU18">
+        <v>0.21253948134835801</v>
+      </c>
+      <c r="CV18">
+        <v>0.227537484490312</v>
+      </c>
+      <c r="CW18">
+        <v>0.25585869397036698</v>
+      </c>
+      <c r="CX18">
+        <v>0.21015316783450499</v>
+      </c>
+      <c r="CY18">
+        <v>0.22880022309254799</v>
+      </c>
+      <c r="CZ18">
+        <v>-4.7663308131242199E-3</v>
+      </c>
+      <c r="DA18">
+        <v>-4.3319212622009197E-2</v>
+      </c>
+      <c r="DB18">
+        <v>-2.83212094800546E-2</v>
+      </c>
+      <c r="DC18">
+        <v>-2.7058470877818701E-2</v>
+      </c>
+      <c r="DD18">
+        <v>-4.5705526135861797E-2</v>
+      </c>
+      <c r="DE18">
+        <v>-1.6260741744190399E-2</v>
+      </c>
+      <c r="DF18">
+        <v>-1.49980031419545E-2</v>
+      </c>
+      <c r="DG18">
+        <v>1.86470552580431E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -6994,8 +7723,47 @@
       <c r="CT19" s="2">
         <v>-0.1961861452</v>
       </c>
+      <c r="CU19">
+        <v>0.30696640536189002</v>
+      </c>
+      <c r="CV19">
+        <v>0.29056982032488998</v>
+      </c>
+      <c r="CW19">
+        <v>0.30336897366214499</v>
+      </c>
+      <c r="CX19">
+        <v>0.30574245750904</v>
+      </c>
+      <c r="CY19">
+        <v>0.30899363989010398</v>
+      </c>
+      <c r="CZ19">
+        <v>2.06213323898347E-3</v>
+      </c>
+      <c r="DA19">
+        <v>3.5974316997453501E-3</v>
+      </c>
+      <c r="DB19">
+        <v>-1.2799153337255099E-2</v>
+      </c>
+      <c r="DC19">
+        <v>5.6246662279590904E-3</v>
+      </c>
+      <c r="DD19">
+        <v>2.3734838468953902E-3</v>
+      </c>
+      <c r="DE19">
+        <v>-2.0272345282137299E-3</v>
+      </c>
+      <c r="DF19">
+        <v>1.6396585037000401E-2</v>
+      </c>
+      <c r="DG19">
+        <v>3.2511823810636902E-3</v>
+      </c>
     </row>
-    <row r="20" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -7308,8 +8076,47 @@
       <c r="CT20" s="2">
         <v>0.54866761310000001</v>
       </c>
+      <c r="CU20">
+        <v>0.23650924318644601</v>
+      </c>
+      <c r="CV20">
+        <v>0.23949521486974801</v>
+      </c>
+      <c r="CW20">
+        <v>0.26371218028361898</v>
+      </c>
+      <c r="CX20">
+        <v>0.255010404034692</v>
+      </c>
+      <c r="CY20">
+        <v>0.24415008858522899</v>
+      </c>
+      <c r="CZ20">
+        <v>-4.3293797091662001E-3</v>
+      </c>
+      <c r="DA20">
+        <v>-2.7202937097172201E-2</v>
+      </c>
+      <c r="DB20">
+        <v>-2.4216965413870601E-2</v>
+      </c>
+      <c r="DC20">
+        <v>-1.9562091698389801E-2</v>
+      </c>
+      <c r="DD20">
+        <v>-8.7017762489267608E-3</v>
+      </c>
+      <c r="DE20">
+        <v>-7.6408453987823997E-3</v>
+      </c>
+      <c r="DF20">
+        <v>-2.9859716833016102E-3</v>
+      </c>
+      <c r="DG20">
+        <v>-1.0860315449463E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -7622,8 +8429,47 @@
       <c r="CT21" s="2">
         <v>-0.53163988539999996</v>
       </c>
+      <c r="CU21">
+        <v>0.31192951760749499</v>
+      </c>
+      <c r="CV21">
+        <v>0.316161317030491</v>
+      </c>
+      <c r="CW21">
+        <v>0.30807536066276903</v>
+      </c>
+      <c r="CX21">
+        <v>0.30272618021990599</v>
+      </c>
+      <c r="CY21">
+        <v>0.31385727528686402</v>
+      </c>
+      <c r="CZ21">
+        <v>1.1810976580558701E-3</v>
+      </c>
+      <c r="DA21">
+        <v>3.8541569447261199E-3</v>
+      </c>
+      <c r="DB21">
+        <v>8.0859563677222399E-3</v>
+      </c>
+      <c r="DC21">
+        <v>5.7819146240944896E-3</v>
+      </c>
+      <c r="DD21">
+        <v>-5.3491804428631396E-3</v>
+      </c>
+      <c r="DE21">
+        <v>-1.92775767936836E-3</v>
+      </c>
+      <c r="DF21">
+        <v>-4.23179942299611E-3</v>
+      </c>
+      <c r="DG21">
+        <v>1.11310950669576E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
@@ -7936,8 +8782,47 @@
       <c r="CT22" s="2">
         <v>-9.2139182639999997E-2</v>
       </c>
+      <c r="CU22">
+        <v>0.276945968158543</v>
+      </c>
+      <c r="CV22">
+        <v>0.27892927033826698</v>
+      </c>
+      <c r="CW22">
+        <v>0.27071501815225901</v>
+      </c>
+      <c r="CX22">
+        <v>0.27823677496053201</v>
+      </c>
+      <c r="CY22">
+        <v>0.29237708583241301</v>
+      </c>
+      <c r="CZ22">
+        <v>2.8607161698996002E-3</v>
+      </c>
+      <c r="DA22">
+        <v>6.2309500062838197E-3</v>
+      </c>
+      <c r="DB22">
+        <v>8.2142521860077908E-3</v>
+      </c>
+      <c r="DC22">
+        <v>2.1662067680153899E-2</v>
+      </c>
+      <c r="DD22">
+        <v>7.5217568082734899E-3</v>
+      </c>
+      <c r="DE22">
+        <v>-1.54311176738701E-2</v>
+      </c>
+      <c r="DF22">
+        <v>-1.9833021797239698E-3</v>
+      </c>
+      <c r="DG22">
+        <v>1.41403108718805E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
@@ -8250,8 +9135,47 @@
       <c r="CT23" s="2">
         <v>-0.1148453153</v>
       </c>
+      <c r="CU23">
+        <v>0.31653699734078999</v>
+      </c>
+      <c r="CV23">
+        <v>0.29115420039033701</v>
+      </c>
+      <c r="CW23">
+        <v>0.28149277151260299</v>
+      </c>
+      <c r="CX23">
+        <v>0.31675721331794099</v>
+      </c>
+      <c r="CY23">
+        <v>0.31341367367713202</v>
+      </c>
+      <c r="CZ23">
+        <v>6.3574560930256801E-3</v>
+      </c>
+      <c r="DA23">
+        <v>3.5044225828187302E-2</v>
+      </c>
+      <c r="DB23">
+        <v>9.6614288777345791E-3</v>
+      </c>
+      <c r="DC23">
+        <v>3.1920902164529197E-2</v>
+      </c>
+      <c r="DD23">
+        <v>3.5264441805338699E-2</v>
+      </c>
+      <c r="DE23">
+        <v>3.1233236636580802E-3</v>
+      </c>
+      <c r="DF23">
+        <v>2.5382796950452698E-2</v>
+      </c>
+      <c r="DG23">
+        <v>-3.3435396408094602E-3</v>
+      </c>
     </row>
-    <row r="24" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
@@ -8564,8 +9488,47 @@
       <c r="CT24" s="2">
         <v>0.71654977040000001</v>
       </c>
+      <c r="CU24">
+        <v>0.29694211028981898</v>
+      </c>
+      <c r="CV24">
+        <v>0.239452081179479</v>
+      </c>
+      <c r="CW24">
+        <v>0.219973833620315</v>
+      </c>
+      <c r="CX24">
+        <v>0.22913358637015299</v>
+      </c>
+      <c r="CY24">
+        <v>0.25394911135663201</v>
+      </c>
+      <c r="CZ24">
+        <v>1.38035077501886E-2</v>
+      </c>
+      <c r="DA24">
+        <v>7.6968276669504093E-2</v>
+      </c>
+      <c r="DB24">
+        <v>1.9478247559163699E-2</v>
+      </c>
+      <c r="DC24">
+        <v>3.3975277736317297E-2</v>
+      </c>
+      <c r="DD24">
+        <v>9.1597527498379298E-3</v>
+      </c>
+      <c r="DE24">
+        <v>4.2992998933186699E-2</v>
+      </c>
+      <c r="DF24">
+        <v>5.7490029110340402E-2</v>
+      </c>
+      <c r="DG24">
+        <v>2.48155249864794E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -8878,8 +9841,47 @@
       <c r="CT25" s="2">
         <v>-0.2174714345</v>
       </c>
+      <c r="CU25">
+        <v>0.33442128088790901</v>
+      </c>
+      <c r="CV25">
+        <v>0.31636660569347402</v>
+      </c>
+      <c r="CW25">
+        <v>0.26959392149001299</v>
+      </c>
+      <c r="CX25">
+        <v>0.31192002794705298</v>
+      </c>
+      <c r="CY25">
+        <v>0.32269746973179197</v>
+      </c>
+      <c r="CZ25">
+        <v>1.04830731870606E-2</v>
+      </c>
+      <c r="DA25">
+        <v>6.4827359397895606E-2</v>
+      </c>
+      <c r="DB25">
+        <v>4.6772684203460799E-2</v>
+      </c>
+      <c r="DC25">
+        <v>5.3103548241779201E-2</v>
+      </c>
+      <c r="DD25">
+        <v>4.23261064570397E-2</v>
+      </c>
+      <c r="DE25">
+        <v>1.17238111561164E-2</v>
+      </c>
+      <c r="DF25">
+        <v>1.8054675194434801E-2</v>
+      </c>
+      <c r="DG25">
+        <v>1.0777441784739401E-2</v>
+      </c>
     </row>
-    <row r="26" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -9192,8 +10194,47 @@
       <c r="CT26" s="2">
         <v>-0.30770898070000002</v>
       </c>
+      <c r="CU26">
+        <v>0.35309921624138901</v>
+      </c>
+      <c r="CV26">
+        <v>0.38635392149444597</v>
+      </c>
+      <c r="CW26">
+        <v>0.370830671745352</v>
+      </c>
+      <c r="CX26">
+        <v>0.38956117839552401</v>
+      </c>
+      <c r="CY26">
+        <v>0.38565342366928201</v>
+      </c>
+      <c r="CZ26">
+        <v>-2.8622259685237698E-3</v>
+      </c>
+      <c r="DA26">
+        <v>-1.7731455503962899E-2</v>
+      </c>
+      <c r="DB26">
+        <v>1.5523249749094199E-2</v>
+      </c>
+      <c r="DC26">
+        <v>1.48227519239299E-2</v>
+      </c>
+      <c r="DD26">
+        <v>1.8730506650172101E-2</v>
+      </c>
+      <c r="DE26">
+        <v>-3.2554207427892799E-2</v>
+      </c>
+      <c r="DF26">
+        <v>-3.3254705253057099E-2</v>
+      </c>
+      <c r="DG26">
+        <v>-3.9077547262422697E-3</v>
+      </c>
     </row>
-    <row r="27" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -9506,8 +10547,47 @@
       <c r="CT27" s="2">
         <v>1.1090153789999999</v>
       </c>
+      <c r="CU27">
+        <v>0.309480648895259</v>
+      </c>
+      <c r="CV27">
+        <v>0.32675396429840398</v>
+      </c>
+      <c r="CW27">
+        <v>0.308012943074572</v>
+      </c>
+      <c r="CX27">
+        <v>0.32442380778957097</v>
+      </c>
+      <c r="CY27">
+        <v>0.30053509975550602</v>
+      </c>
+      <c r="CZ27">
+        <v>-3.36944006682772E-3</v>
+      </c>
+      <c r="DA27">
+        <v>1.46770582068711E-3</v>
+      </c>
+      <c r="DB27">
+        <v>1.8741021223831901E-2</v>
+      </c>
+      <c r="DC27">
+        <v>-7.4778433190658602E-3</v>
+      </c>
+      <c r="DD27">
+        <v>1.64108647149987E-2</v>
+      </c>
+      <c r="DE27">
+        <v>8.9455491397529806E-3</v>
+      </c>
+      <c r="DF27">
+        <v>-1.72733154031448E-2</v>
+      </c>
+      <c r="DG27">
+        <v>-2.38887080340646E-2</v>
+      </c>
     </row>
-    <row r="28" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
@@ -9820,8 +10900,47 @@
       <c r="CT28" s="2">
         <v>-0.41720973849999998</v>
       </c>
+      <c r="CU28">
+        <v>0.31061711788061003</v>
+      </c>
+      <c r="CV28">
+        <v>0.327592697198269</v>
+      </c>
+      <c r="CW28">
+        <v>0.31018091001897102</v>
+      </c>
+      <c r="CX28">
+        <v>0.25669941294472598</v>
+      </c>
+      <c r="CY28">
+        <v>0.31103491142857798</v>
+      </c>
+      <c r="CZ28">
+        <v>2.7607234598170599E-3</v>
+      </c>
+      <c r="DA28">
+        <v>4.36207861639559E-4</v>
+      </c>
+      <c r="DB28">
+        <v>1.7411787179298699E-2</v>
+      </c>
+      <c r="DC28">
+        <v>8.5400140960700799E-4</v>
+      </c>
+      <c r="DD28">
+        <v>-5.3481497074244502E-2</v>
+      </c>
+      <c r="DE28">
+        <v>-4.1779354796744802E-4</v>
+      </c>
+      <c r="DF28">
+        <v>-1.6975579317659101E-2</v>
+      </c>
+      <c r="DG28">
+        <v>5.4335498483851503E-2</v>
+      </c>
     </row>
-    <row r="29" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
@@ -10134,8 +11253,47 @@
       <c r="CT29" s="2">
         <v>-9.8361420590000002E-3</v>
       </c>
+      <c r="CU29">
+        <v>0.24043969999911399</v>
+      </c>
+      <c r="CV29">
+        <v>0.26800750000256801</v>
+      </c>
+      <c r="CW29">
+        <v>0.27326109999921699</v>
+      </c>
+      <c r="CX29">
+        <v>0.28887400000166902</v>
+      </c>
+      <c r="CY29">
+        <v>0.258038300002226</v>
+      </c>
+      <c r="CZ29">
+        <v>-7.6034071428564103E-3</v>
+      </c>
+      <c r="DA29">
+        <v>-3.2821400000102502E-2</v>
+      </c>
+      <c r="DB29">
+        <v>-5.2535999966494204E-3</v>
+      </c>
+      <c r="DC29">
+        <v>-1.52227999969909E-2</v>
+      </c>
+      <c r="DD29">
+        <v>1.5612900002451999E-2</v>
+      </c>
+      <c r="DE29">
+        <v>-1.75986000031116E-2</v>
+      </c>
+      <c r="DF29">
+        <v>-2.7567800003453099E-2</v>
+      </c>
+      <c r="DG29">
+        <v>-3.0835699999443002E-2</v>
+      </c>
     </row>
-    <row r="30" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
@@ -10448,8 +11606,47 @@
       <c r="CT30" s="2">
         <v>-0.63191312550000001</v>
       </c>
+      <c r="CU30">
+        <v>0.30175958454492502</v>
+      </c>
+      <c r="CV30">
+        <v>0.276141779846511</v>
+      </c>
+      <c r="CW30">
+        <v>0.29592167254304502</v>
+      </c>
+      <c r="CX30">
+        <v>0.285913090308895</v>
+      </c>
+      <c r="CY30">
+        <v>0.27923204848775601</v>
+      </c>
+      <c r="CZ30">
+        <v>5.7750363027611704E-4</v>
+      </c>
+      <c r="DA30">
+        <v>5.8379120018798797E-3</v>
+      </c>
+      <c r="DB30">
+        <v>-1.97798926965333E-2</v>
+      </c>
+      <c r="DC30">
+        <v>-1.6689624055288701E-2</v>
+      </c>
+      <c r="DD30">
+        <v>-1.00085822341497E-2</v>
+      </c>
+      <c r="DE30">
+        <v>2.25275360571686E-2</v>
+      </c>
+      <c r="DF30">
+        <v>2.56178046984132E-2</v>
+      </c>
+      <c r="DG30">
+        <v>-6.6810418211389298E-3</v>
+      </c>
     </row>
-    <row r="31" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>18</v>
       </c>
@@ -10762,8 +11959,47 @@
       <c r="CT31" s="2">
         <v>0.19399214949999999</v>
       </c>
+      <c r="CU31">
+        <v>0.24958635913208099</v>
+      </c>
+      <c r="CV31">
+        <v>0.25142989447340303</v>
+      </c>
+      <c r="CW31">
+        <v>0.25946936244145002</v>
+      </c>
+      <c r="CX31">
+        <v>0.237753561581484</v>
+      </c>
+      <c r="CY31">
+        <v>0.25313970015849901</v>
+      </c>
+      <c r="CZ31">
+        <v>-1.9071873975918101E-4</v>
+      </c>
+      <c r="DA31">
+        <v>-9.8830033093690803E-3</v>
+      </c>
+      <c r="DB31">
+        <v>-8.03946796804666E-3</v>
+      </c>
+      <c r="DC31">
+        <v>-6.3296622829511701E-3</v>
+      </c>
+      <c r="DD31">
+        <v>-2.1715800859965301E-2</v>
+      </c>
+      <c r="DE31">
+        <v>-3.5533410264179102E-3</v>
+      </c>
+      <c r="DF31">
+        <v>-1.8435353413224201E-3</v>
+      </c>
+      <c r="DG31">
+        <v>1.5386138577014199E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -11076,8 +12312,47 @@
       <c r="CT32" s="2">
         <v>-0.93062408340000002</v>
       </c>
+      <c r="CU32">
+        <v>0.40755706885829501</v>
+      </c>
+      <c r="CV32">
+        <v>0.41934548062272298</v>
+      </c>
+      <c r="CW32">
+        <v>0.43431985168717802</v>
+      </c>
+      <c r="CX32">
+        <v>0.373613651841878</v>
+      </c>
+      <c r="CY32">
+        <v>0.32261203974485397</v>
+      </c>
+      <c r="CZ32">
+        <v>-1.43757584737613E-2</v>
+      </c>
+      <c r="DA32">
+        <v>-2.6762782828882298E-2</v>
+      </c>
+      <c r="DB32">
+        <v>-1.49743710644543E-2</v>
+      </c>
+      <c r="DC32">
+        <v>-0.111707811942324</v>
+      </c>
+      <c r="DD32">
+        <v>-6.0706199845299097E-2</v>
+      </c>
+      <c r="DE32">
+        <v>8.4945029113441706E-2</v>
+      </c>
+      <c r="DF32">
+        <v>-1.1788411764428E-2</v>
+      </c>
+      <c r="DG32">
+        <v>-5.1001612097024897E-2</v>
+      </c>
     </row>
-    <row r="33" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>20</v>
       </c>
@@ -11390,8 +12665,47 @@
       <c r="CT33" s="2">
         <v>-0.30071019450000003</v>
       </c>
+      <c r="CU33">
+        <v>0.29532931579160498</v>
+      </c>
+      <c r="CV33">
+        <v>0.31495051832462101</v>
+      </c>
+      <c r="CW33">
+        <v>0.35074371173686802</v>
+      </c>
+      <c r="CX33">
+        <v>0.29348909223335701</v>
+      </c>
+      <c r="CY33">
+        <v>0.28530619526281897</v>
+      </c>
+      <c r="CZ33">
+        <v>-1.0618286565919E-2</v>
+      </c>
+      <c r="DA33">
+        <v>-5.5414395945262998E-2</v>
+      </c>
+      <c r="DB33">
+        <v>-3.5793193412246099E-2</v>
+      </c>
+      <c r="DC33">
+        <v>-6.5437516474048593E-2</v>
+      </c>
+      <c r="DD33">
+        <v>-5.7254619503510101E-2</v>
+      </c>
+      <c r="DE33">
+        <v>1.00231205287855E-2</v>
+      </c>
+      <c r="DF33">
+        <v>-1.9621202533016899E-2</v>
+      </c>
+      <c r="DG33">
+        <v>-8.1828969705384207E-3</v>
+      </c>
     </row>
-    <row r="34" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -11704,8 +13018,47 @@
       <c r="CT34" s="2">
         <v>-0.28935340040000002</v>
       </c>
+      <c r="CU34">
+        <v>0.25569203210761698</v>
+      </c>
+      <c r="CV34">
+        <v>0.27452464896487</v>
+      </c>
+      <c r="CW34">
+        <v>0.31919694674434101</v>
+      </c>
+      <c r="CX34">
+        <v>0.21977720604627299</v>
+      </c>
+      <c r="CY34">
+        <v>0.27808915924106198</v>
+      </c>
+      <c r="CZ34">
+        <v>-4.6523832716047599E-3</v>
+      </c>
+      <c r="DA34">
+        <v>-6.3504914636723697E-2</v>
+      </c>
+      <c r="DB34">
+        <v>-4.4672297779470599E-2</v>
+      </c>
+      <c r="DC34">
+        <v>-4.11077875032788E-2</v>
+      </c>
+      <c r="DD34">
+        <v>-9.9419740698067402E-2</v>
+      </c>
+      <c r="DE34">
+        <v>-2.23971271334448E-2</v>
+      </c>
+      <c r="DF34">
+        <v>-1.8832616857253001E-2</v>
+      </c>
+      <c r="DG34">
+        <v>5.8311953194788602E-2</v>
+      </c>
     </row>
-    <row r="35" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
@@ -12018,8 +13371,47 @@
       <c r="CT35" s="2">
         <v>0.2381286635</v>
       </c>
+      <c r="CU35">
+        <v>0.27095711999572802</v>
+      </c>
+      <c r="CV35">
+        <v>0.26093404786661201</v>
+      </c>
+      <c r="CW35">
+        <v>0.32185583957470898</v>
+      </c>
+      <c r="CX35">
+        <v>0.29167764727026202</v>
+      </c>
+      <c r="CY35">
+        <v>0.31236949667800201</v>
+      </c>
+      <c r="CZ35">
+        <v>-2.11929578134524E-3</v>
+      </c>
+      <c r="DA35">
+        <v>-5.08987195789814E-2</v>
+      </c>
+      <c r="DB35">
+        <v>-6.0921791708096799E-2</v>
+      </c>
+      <c r="DC35">
+        <v>-9.4863428967073508E-3</v>
+      </c>
+      <c r="DD35">
+        <v>-3.01781923044472E-2</v>
+      </c>
+      <c r="DE35">
+        <v>-4.1412376682274002E-2</v>
+      </c>
+      <c r="DF35">
+        <v>1.00230721291154E-2</v>
+      </c>
+      <c r="DG35">
+        <v>2.0691849407739899E-2</v>
+      </c>
     </row>
-    <row r="36" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>27</v>
       </c>
@@ -12332,8 +13724,47 @@
       <c r="CT36" s="2">
         <v>-0.72131246559999995</v>
       </c>
+      <c r="CU36">
+        <v>0.32115699999849301</v>
+      </c>
+      <c r="CV36">
+        <v>0.32137630000943301</v>
+      </c>
+      <c r="CW36">
+        <v>0.31825130000652202</v>
+      </c>
+      <c r="CX36">
+        <v>0.33935379999456899</v>
+      </c>
+      <c r="CY36">
+        <v>0.32835140000679502</v>
+      </c>
+      <c r="CZ36">
+        <v>1.2743571382348899E-4</v>
+      </c>
+      <c r="DA36">
+        <v>2.90569999197032E-3</v>
+      </c>
+      <c r="DB36">
+        <v>3.12500000291038E-3</v>
+      </c>
+      <c r="DC36">
+        <v>1.01001000002725E-2</v>
+      </c>
+      <c r="DD36">
+        <v>2.1102499988046398E-2</v>
+      </c>
+      <c r="DE36">
+        <v>-7.1944000083021802E-3</v>
+      </c>
+      <c r="DF36">
+        <v>-2.1930001094005999E-4</v>
+      </c>
+      <c r="DG36">
+        <v>-1.10023999877739E-2</v>
+      </c>
     </row>
-    <row r="37" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
@@ -12646,8 +14077,47 @@
       <c r="CT37" s="2">
         <v>0.27465553729999997</v>
       </c>
+      <c r="CU37">
+        <v>0.330868997305515</v>
+      </c>
+      <c r="CV37">
+        <v>0.34617498883744702</v>
+      </c>
+      <c r="CW37">
+        <v>0.32600145443575401</v>
+      </c>
+      <c r="CX37">
+        <v>0.32111776137025999</v>
+      </c>
+      <c r="CY37">
+        <v>0.33702493194141397</v>
+      </c>
+      <c r="CZ37">
+        <v>1.1780142439030499E-3</v>
+      </c>
+      <c r="DA37">
+        <v>4.8675428697606497E-3</v>
+      </c>
+      <c r="DB37">
+        <v>2.0173534401692401E-2</v>
+      </c>
+      <c r="DC37">
+        <v>1.10234775056596E-2</v>
+      </c>
+      <c r="DD37">
+        <v>-4.8836930654942903E-3</v>
+      </c>
+      <c r="DE37">
+        <v>-6.1559346358990297E-3</v>
+      </c>
+      <c r="DF37">
+        <v>-1.53059915319317E-2</v>
+      </c>
+      <c r="DG37">
+        <v>1.59071705711539E-2</v>
+      </c>
     </row>
-    <row r="38" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
@@ -12960,8 +14430,47 @@
       <c r="CT38" s="2">
         <v>0.34599991299999999</v>
       </c>
+      <c r="CU38">
+        <v>0.26031169999623599</v>
+      </c>
+      <c r="CV38">
+        <v>0.24865109997335799</v>
+      </c>
+      <c r="CW38">
+        <v>0.36765630001900701</v>
+      </c>
+      <c r="CX38">
+        <v>0.25837260001571799</v>
+      </c>
+      <c r="CY38">
+        <v>0.27290470001753397</v>
+      </c>
+      <c r="CZ38">
+        <v>-1.25645357142535E-2</v>
+      </c>
+      <c r="DA38">
+        <v>-0.10734460002277001</v>
+      </c>
+      <c r="DB38">
+        <v>-0.119005200045648</v>
+      </c>
+      <c r="DC38">
+        <v>-9.4751600001472897E-2</v>
+      </c>
+      <c r="DD38">
+        <v>-0.10928370000328801</v>
+      </c>
+      <c r="DE38">
+        <v>-1.25930000212974E-2</v>
+      </c>
+      <c r="DF38">
+        <v>1.1660600022878401E-2</v>
+      </c>
+      <c r="DG38">
+        <v>1.45321000018157E-2</v>
+      </c>
     </row>
-    <row r="39" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>25</v>
       </c>
@@ -13274,8 +14783,47 @@
       <c r="CT39" s="2">
         <v>-0.12923029820000001</v>
       </c>
+      <c r="CU39">
+        <v>0.29838525387458498</v>
+      </c>
+      <c r="CV39">
+        <v>0.26985317224171002</v>
+      </c>
+      <c r="CW39">
+        <v>0.28624831972410902</v>
+      </c>
+      <c r="CX39">
+        <v>0.30872106592869297</v>
+      </c>
+      <c r="CY39">
+        <v>0.28544971602968799</v>
+      </c>
+      <c r="CZ39">
+        <v>1.18564729928038E-3</v>
+      </c>
+      <c r="DA39">
+        <v>1.2136934150476E-2</v>
+      </c>
+      <c r="DB39">
+        <v>-1.63951474823988E-2</v>
+      </c>
+      <c r="DC39">
+        <v>-7.9860369442030701E-4</v>
+      </c>
+      <c r="DD39">
+        <v>2.2472746204584799E-2</v>
+      </c>
+      <c r="DE39">
+        <v>1.2935537844896299E-2</v>
+      </c>
+      <c r="DF39">
+        <v>2.8532081632874899E-2</v>
+      </c>
+      <c r="DG39">
+        <v>-2.32713498990051E-2</v>
+      </c>
     </row>
-    <row r="40" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>24</v>
       </c>
@@ -13588,8 +15136,47 @@
       <c r="CT40" s="2">
         <v>-0.36050643989999998</v>
       </c>
+      <c r="CU40">
+        <v>0.26389229999767799</v>
+      </c>
+      <c r="CV40">
+        <v>0.25869560000137398</v>
+      </c>
+      <c r="CW40">
+        <v>0.27253230000496798</v>
+      </c>
+      <c r="CX40">
+        <v>0.27097800000046801</v>
+      </c>
+      <c r="CY40">
+        <v>0.262517000002844</v>
+      </c>
+      <c r="CZ40">
+        <v>-1.5656857150523501E-3</v>
+      </c>
+      <c r="DA40">
+        <v>-8.6400000072899205E-3</v>
+      </c>
+      <c r="DB40">
+        <v>-1.3836700003594099E-2</v>
+      </c>
+      <c r="DC40">
+        <v>-1.0015300002123599E-2</v>
+      </c>
+      <c r="DD40">
+        <v>-1.5543000044999601E-3</v>
+      </c>
+      <c r="DE40">
+        <v>1.37529999483376E-3</v>
+      </c>
+      <c r="DF40">
+        <v>5.19669999630423E-3</v>
+      </c>
+      <c r="DG40">
+        <v>-8.4609999976237305E-3</v>
+      </c>
     </row>
-    <row r="41" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -13902,8 +15489,47 @@
       <c r="CT41" s="2">
         <v>0.59186078990000002</v>
       </c>
+      <c r="CU41">
+        <v>0.27478430001065102</v>
+      </c>
+      <c r="CV41">
+        <v>0.30509630002779797</v>
+      </c>
+      <c r="CW41">
+        <v>0.42112389998510402</v>
+      </c>
+      <c r="CX41">
+        <v>0.43343699997058099</v>
+      </c>
+      <c r="CY41">
+        <v>0.34199659997830101</v>
+      </c>
+      <c r="CZ41">
+        <v>-2.4801378570762998E-2</v>
+      </c>
+      <c r="DA41">
+        <v>-0.14633959997445301</v>
+      </c>
+      <c r="DB41">
+        <v>-0.11602759995730499</v>
+      </c>
+      <c r="DC41">
+        <v>-7.9127300006803097E-2</v>
+      </c>
+      <c r="DD41">
+        <v>1.23130999854765E-2</v>
+      </c>
+      <c r="DE41">
+        <v>-6.7212299967650296E-2</v>
+      </c>
+      <c r="DF41">
+        <v>-3.0312000017147501E-2</v>
+      </c>
+      <c r="DG41">
+        <v>-9.1440399992279695E-2</v>
+      </c>
     </row>
-    <row r="42" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>31</v>
       </c>
@@ -14216,8 +15842,47 @@
       <c r="CT42" s="2">
         <v>-0.2406223552</v>
       </c>
+      <c r="CU42">
+        <v>0.25526109989732498</v>
+      </c>
+      <c r="CV42">
+        <v>0.32960830000229102</v>
+      </c>
+      <c r="CW42">
+        <v>0.50983945000916697</v>
+      </c>
+      <c r="CX42">
+        <v>0.31709309993311702</v>
+      </c>
+      <c r="CY42">
+        <v>0.32746299984864802</v>
+      </c>
+      <c r="CZ42">
+        <v>-3.5780864318699701E-2</v>
+      </c>
+      <c r="DA42">
+        <v>-0.25457835011184199</v>
+      </c>
+      <c r="DB42">
+        <v>-0.18023115000687501</v>
+      </c>
+      <c r="DC42">
+        <v>-0.18237645016051801</v>
+      </c>
+      <c r="DD42">
+        <v>-0.19274635007604901</v>
+      </c>
+      <c r="DE42">
+        <v>-7.2201899951323797E-2</v>
+      </c>
+      <c r="DF42">
+        <v>-7.4347200104966704E-2</v>
+      </c>
+      <c r="DG42">
+        <v>1.03698999155312E-2</v>
+      </c>
     </row>
-    <row r="43" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>22</v>
       </c>
@@ -14530,8 +16195,47 @@
       <c r="CT43" s="2">
         <v>-0.28642412070000001</v>
       </c>
+      <c r="CU43">
+        <v>0.25166589999571398</v>
+      </c>
+      <c r="CV43">
+        <v>0.26142870000330698</v>
+      </c>
+      <c r="CW43">
+        <v>0.26647029997548</v>
+      </c>
+      <c r="CX43">
+        <v>0.25061879999702702</v>
+      </c>
+      <c r="CY43">
+        <v>0.240791800024453</v>
+      </c>
+      <c r="CZ43">
+        <v>-4.2909071364972103E-3</v>
+      </c>
+      <c r="DA43">
+        <v>-1.4804399979766399E-2</v>
+      </c>
+      <c r="DB43">
+        <v>-5.0415999721735699E-3</v>
+      </c>
+      <c r="DC43">
+        <v>-2.5678499951027299E-2</v>
+      </c>
+      <c r="DD43">
+        <v>-1.58514999784529E-2</v>
+      </c>
+      <c r="DE43">
+        <v>1.0874099971260799E-2</v>
+      </c>
+      <c r="DF43">
+        <v>-9.7628000075928797E-3</v>
+      </c>
+      <c r="DG43">
+        <v>-9.8269999725744094E-3</v>
+      </c>
     </row>
-    <row r="44" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
@@ -14844,8 +16548,47 @@
       <c r="CT44" s="2">
         <v>0.4606249322</v>
       </c>
+      <c r="CU44">
+        <v>0.309154100017622</v>
+      </c>
+      <c r="CV44">
+        <v>0.35540389991365301</v>
+      </c>
+      <c r="CW44">
+        <v>0.44437369983643199</v>
+      </c>
+      <c r="CX44">
+        <v>0.38728519994765498</v>
+      </c>
+      <c r="CY44">
+        <v>0.32651179982349199</v>
+      </c>
+      <c r="CZ44">
+        <v>-2.5721764275138899E-2</v>
+      </c>
+      <c r="DA44">
+        <v>-0.13521959981880999</v>
+      </c>
+      <c r="DB44">
+        <v>-8.8969799922779202E-2</v>
+      </c>
+      <c r="DC44">
+        <v>-0.11786190001294</v>
+      </c>
+      <c r="DD44">
+        <v>-5.7088499888777698E-2</v>
+      </c>
+      <c r="DE44">
+        <v>-1.73576998058706E-2</v>
+      </c>
+      <c r="DF44">
+        <v>-4.6249799896031597E-2</v>
+      </c>
+      <c r="DG44">
+        <v>-6.0773400124162401E-2</v>
+      </c>
     </row>
-    <row r="45" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
@@ -15158,8 +16901,47 @@
       <c r="CT45" s="2">
         <v>-0.63439562790000004</v>
       </c>
+      <c r="CU45">
+        <v>0.26531110005453201</v>
+      </c>
+      <c r="CV45">
+        <v>0.30091230000834901</v>
+      </c>
+      <c r="CW45">
+        <v>0.31645939999725597</v>
+      </c>
+      <c r="CX45">
+        <v>0.37248519994318402</v>
+      </c>
+      <c r="CY45">
+        <v>0.26834149996284301</v>
+      </c>
+      <c r="CZ45">
+        <v>-1.7072221422235301E-2</v>
+      </c>
+      <c r="DA45">
+        <v>-5.11482999427244E-2</v>
+      </c>
+      <c r="DB45">
+        <v>-1.5547099988907499E-2</v>
+      </c>
+      <c r="DC45">
+        <v>-4.81179000344127E-2</v>
+      </c>
+      <c r="DD45">
+        <v>5.6025799945928101E-2</v>
+      </c>
+      <c r="DE45">
+        <v>-3.0303999083116599E-3</v>
+      </c>
+      <c r="DF45">
+        <v>-3.5601199953816803E-2</v>
+      </c>
+      <c r="DG45">
+        <v>-0.10414369998034</v>
+      </c>
     </row>
-    <row r="46" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>29</v>
       </c>
@@ -15472,8 +17254,47 @@
       <c r="CT46" s="2">
         <v>-1.2903293689999999</v>
       </c>
+      <c r="CU46">
+        <v>0.29868469992652502</v>
+      </c>
+      <c r="CV46">
+        <v>0.27217550016939601</v>
+      </c>
+      <c r="CW46">
+        <v>0.299600899685174</v>
+      </c>
+      <c r="CX46">
+        <v>0.30233040032908298</v>
+      </c>
+      <c r="CY46">
+        <v>0.27748880023136702</v>
+      </c>
+      <c r="CZ46">
+        <v>-1.5257642537887699E-3</v>
+      </c>
+      <c r="DA46">
+        <v>-9.1619975864887205E-4</v>
+      </c>
+      <c r="DB46">
+        <v>-2.7425399515777799E-2</v>
+      </c>
+      <c r="DC46">
+        <v>-2.2112099453806801E-2</v>
+      </c>
+      <c r="DD46">
+        <v>2.7295006439089701E-3</v>
+      </c>
+      <c r="DE46">
+        <v>2.1195899695158001E-2</v>
+      </c>
+      <c r="DF46">
+        <v>2.6509199757128898E-2</v>
+      </c>
+      <c r="DG46">
+        <v>-2.4841600097715799E-2</v>
+      </c>
     </row>
-    <row r="47" spans="1:98" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:111" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>35</v>
       </c>
@@ -15785,6 +17606,45 @@
       </c>
       <c r="CT47" s="2">
         <v>0.22453609420000001</v>
+      </c>
+      <c r="CU47">
+        <v>0.35358945000916697</v>
+      </c>
+      <c r="CV47">
+        <v>0.45092039974406301</v>
+      </c>
+      <c r="CW47">
+        <v>0.37348589999601201</v>
+      </c>
+      <c r="CX47">
+        <v>0.44888090016320298</v>
+      </c>
+      <c r="CY47">
+        <v>0.34719959995709299</v>
+      </c>
+      <c r="CZ47">
+        <v>-1.7513928569054999E-2</v>
+      </c>
+      <c r="DA47">
+        <v>-1.9896449986845199E-2</v>
+      </c>
+      <c r="DB47">
+        <v>7.7434499748051097E-2</v>
+      </c>
+      <c r="DC47">
+        <v>-2.6286300038918801E-2</v>
+      </c>
+      <c r="DD47">
+        <v>7.5395000167191001E-2</v>
+      </c>
+      <c r="DE47">
+        <v>6.3898500520735901E-3</v>
+      </c>
+      <c r="DF47">
+        <v>-9.7330949734896394E-2</v>
+      </c>
+      <c r="DG47">
+        <v>-0.10168130020610899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test changes to plot
</commit_message>
<xml_diff>
--- a/code/total_df_n46.xlsx
+++ b/code/total_df_n46.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-mid-clean/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C98E7FB-CD07-EF42-8251-9497A8BD92EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9555B970-7F64-5642-8BE5-0DAC00F74835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1220" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="208">
   <si>
     <t>Sub</t>
   </si>
@@ -651,6 +651,15 @@
   </si>
   <si>
     <t>LG_N_split</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Low (-1SD)</t>
+  </si>
+  <si>
+    <t>High (+1SD)</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1083,10 @@
   <dimension ref="A1:DI47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CW21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DE40" sqref="DE40"/>
+      <selection pane="bottomRight" activeCell="DC58" sqref="DC58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1768,7 +1777,7 @@
         <v>-0.25457835011184199</v>
       </c>
       <c r="DB2" t="s">
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="DC2">
         <v>-1.16798956878483E-2</v>
@@ -2128,7 +2137,7 @@
         <v>-0.14633959997445301</v>
       </c>
       <c r="DB3" t="s">
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="DC3">
         <v>2.09843575867125E-2</v>
@@ -2149,7 +2158,7 @@
         <v>-8.1175750718102693E-2</v>
       </c>
       <c r="DI3">
-        <f t="shared" ref="DI3:DI47" si="0">CU3-CY3</f>
+        <f>CU3-CY3</f>
         <v>-6.7212299967649991E-2</v>
       </c>
     </row>
@@ -2488,7 +2497,7 @@
         <v>-0.13521959981880999</v>
       </c>
       <c r="DB4" t="s">
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="DC4">
         <v>1.6252809669822399E-2</v>
@@ -2509,7 +2518,7 @@
         <v>-3.9855759358033503E-2</v>
       </c>
       <c r="DI4">
-        <f t="shared" si="0"/>
+        <f>CU4-CY4</f>
         <v>-1.7357699805869986E-2</v>
       </c>
     </row>
@@ -2848,7 +2857,7 @@
         <v>-0.10734460002277001</v>
       </c>
       <c r="DB5" t="s">
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="DC5">
         <v>-1.6335683467332201E-2</v>
@@ -2869,7 +2878,7 @@
         <v>-2.06871766713447E-2</v>
       </c>
       <c r="DI5">
-        <f t="shared" si="0"/>
+        <f>CU5-CY5</f>
         <v>-1.2593000021297984E-2</v>
       </c>
     </row>
@@ -3208,7 +3217,7 @@
         <v>-6.3504914636723697E-2</v>
       </c>
       <c r="DB6" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC6">
         <v>-7.8944207634776796E-3</v>
@@ -3229,7 +3238,7 @@
         <v>5.3202022099867402E-3</v>
       </c>
       <c r="DI6">
-        <f t="shared" si="0"/>
+        <f>CU6-CY6</f>
         <v>-2.2397127133444994E-2</v>
       </c>
     </row>
@@ -3568,7 +3577,7 @@
         <v>-5.5414395945262998E-2</v>
       </c>
       <c r="DB7" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC7">
         <v>1.55828368733637E-2</v>
@@ -3589,7 +3598,7 @@
         <v>-1.8720957916229901E-2</v>
       </c>
       <c r="DI7">
-        <f t="shared" si="0"/>
+        <f>CU7-CY7</f>
         <v>1.0023120528786011E-2</v>
       </c>
     </row>
@@ -3928,7 +3937,7 @@
         <v>-5.11482999427244E-2</v>
       </c>
       <c r="DB8" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC8">
         <v>-1.18083389243111E-2</v>
@@ -3949,7 +3958,7 @@
         <v>-4.9816477112471997E-3</v>
       </c>
       <c r="DI8">
-        <f t="shared" si="0"/>
+        <f>CU8-CY8</f>
         <v>-3.0303999083109989E-3</v>
       </c>
     </row>
@@ -4288,7 +4297,7 @@
         <v>-5.08987195789814E-2</v>
       </c>
       <c r="DB9" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC9">
         <v>-5.0698698614723897E-2</v>
@@ -4309,7 +4318,7 @@
         <v>-2.9760382836684501E-2</v>
       </c>
       <c r="DI9">
-        <f t="shared" si="0"/>
+        <f>CU9-CY9</f>
         <v>-4.1412376682273988E-2</v>
       </c>
     </row>
@@ -4648,7 +4657,7 @@
         <v>-4.3319212622009197E-2</v>
       </c>
       <c r="DB10" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC10">
         <v>-1.1424083008023399E-2</v>
@@ -4669,7 +4678,7 @@
         <v>-3.0062780534535701E-2</v>
       </c>
       <c r="DI10">
-        <f t="shared" si="0"/>
+        <f>CU10-CY10</f>
         <v>-1.6260741744189983E-2</v>
       </c>
     </row>
@@ -5008,7 +5017,7 @@
         <v>-4.2208238213788697E-2</v>
       </c>
       <c r="DB11" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC11">
         <v>2.6066434336826198E-2</v>
@@ -5029,7 +5038,7 @@
         <v>-4.7980454284697702E-2</v>
       </c>
       <c r="DI11">
-        <f t="shared" si="0"/>
+        <f>CU11-CY11</f>
         <v>-1.8702045723331007E-2</v>
       </c>
     </row>
@@ -5368,7 +5377,7 @@
         <v>-3.5077569467830402E-2</v>
       </c>
       <c r="DB12" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC12">
         <v>-8.8674982544034698E-4</v>
@@ -5389,7 +5398,7 @@
         <v>-5.4749071132391596E-3</v>
       </c>
       <c r="DI12">
-        <f t="shared" si="0"/>
+        <f>CU12-CY12</f>
         <v>-4.6165993087925017E-2</v>
       </c>
     </row>
@@ -5728,7 +5737,7 @@
         <v>-3.2821400000102502E-2</v>
       </c>
       <c r="DB13" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC13">
         <v>2.9919088934548199E-2</v>
@@ -5749,7 +5758,7 @@
         <v>-3.1870396283920799E-2</v>
       </c>
       <c r="DI13">
-        <f t="shared" si="0"/>
+        <f>CU13-CY13</f>
         <v>-1.7598600003112003E-2</v>
       </c>
     </row>
@@ -6088,7 +6097,7 @@
         <v>-2.7202937097172201E-2</v>
       </c>
       <c r="DB14" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC14">
         <v>4.2111438873689601E-2</v>
@@ -6109,7 +6118,7 @@
         <v>-9.2224475170951295E-2</v>
       </c>
       <c r="DI14">
-        <f t="shared" si="0"/>
+        <f>CU14-CY14</f>
         <v>-7.6408453987829861E-3</v>
       </c>
     </row>
@@ -6448,7 +6457,7 @@
         <v>-2.6762782828882298E-2</v>
       </c>
       <c r="DB15" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC15">
         <v>-3.5798626782707198E-2</v>
@@ -6469,7 +6478,7 @@
         <v>-4.31315666719456E-2</v>
       </c>
       <c r="DI15">
-        <f t="shared" si="0"/>
+        <f>CU15-CY15</f>
         <v>8.494502911344104E-2</v>
       </c>
     </row>
@@ -6808,7 +6817,7 @@
         <v>-2.6752384321298402E-2</v>
       </c>
       <c r="DB16" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC16">
         <v>6.2691368275409297E-3</v>
@@ -6829,7 +6838,7 @@
         <v>1.3767045606982701E-2</v>
       </c>
       <c r="DI16">
-        <f t="shared" si="0"/>
+        <f>CU16-CY16</f>
         <v>-2.9366146191029951E-3</v>
       </c>
     </row>
@@ -7168,7 +7177,7 @@
         <v>-2.3400558333378198E-2</v>
       </c>
       <c r="DB17" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC17">
         <v>-3.4930104171507902E-2</v>
@@ -7189,7 +7198,7 @@
         <v>4.2077567050000597E-2</v>
       </c>
       <c r="DI17">
-        <f t="shared" si="0"/>
+        <f>CU17-CY17</f>
         <v>-4.0481117321200522E-4</v>
       </c>
     </row>
@@ -7528,7 +7537,7 @@
         <v>-2.2780944127589398E-2</v>
       </c>
       <c r="DB18" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC18">
         <v>-2.83212094800546E-2</v>
@@ -7549,7 +7558,7 @@
         <v>1.86470552580431E-2</v>
       </c>
       <c r="DI18">
-        <f t="shared" si="0"/>
+        <f>CU18-CY18</f>
         <v>3.7174064782448002E-2</v>
       </c>
     </row>
@@ -7888,7 +7897,7 @@
         <v>-1.9896449986845199E-2</v>
       </c>
       <c r="DB19" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC19">
         <v>-1.2799153337255099E-2</v>
@@ -7909,7 +7918,7 @@
         <v>3.2511823810636902E-3</v>
       </c>
       <c r="DI19">
-        <f t="shared" si="0"/>
+        <f>CU19-CY19</f>
         <v>6.3898500520739865E-3</v>
       </c>
     </row>
@@ -8248,7 +8257,7 @@
         <v>-1.8544630490396199E-2</v>
       </c>
       <c r="DB20" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC20">
         <v>-2.4216965413870601E-2</v>
@@ -8269,7 +8278,7 @@
         <v>-1.0860315449463E-2</v>
       </c>
       <c r="DI20">
-        <f t="shared" si="0"/>
+        <f>CU20-CY20</f>
         <v>-1.2112331582102009E-2</v>
       </c>
     </row>
@@ -8608,7 +8617,7 @@
         <v>-1.7731455503962899E-2</v>
       </c>
       <c r="DB21" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC21">
         <v>8.0859563677222399E-3</v>
@@ -8629,7 +8638,7 @@
         <v>1.11310950669576E-2</v>
       </c>
       <c r="DI21">
-        <f t="shared" si="0"/>
+        <f>CU21-CY21</f>
         <v>-3.2554207427893E-2</v>
       </c>
     </row>
@@ -8968,7 +8977,7 @@
         <v>-1.7511503596324401E-2</v>
       </c>
       <c r="DB22" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC22">
         <v>8.2142521860077908E-3</v>
@@ -8989,7 +8998,7 @@
         <v>1.41403108718805E-2</v>
       </c>
       <c r="DI22">
-        <f t="shared" si="0"/>
+        <f>CU22-CY22</f>
         <v>-6.4615916926402672E-4</v>
       </c>
     </row>
@@ -9328,7 +9337,7 @@
         <v>-1.70621656197909E-2</v>
       </c>
       <c r="DB23" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC23">
         <v>9.6614288777345791E-3</v>
@@ -9349,7 +9358,7 @@
         <v>-3.3435396408094602E-3</v>
       </c>
       <c r="DI23">
-        <f t="shared" si="0"/>
+        <f>CU23-CY23</f>
         <v>1.7301852794839867E-3</v>
       </c>
     </row>
@@ -9688,7 +9697,7 @@
         <v>-1.49652045220136E-2</v>
       </c>
       <c r="DB24" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC24">
         <v>1.9478247559163699E-2</v>
@@ -9709,7 +9718,7 @@
         <v>2.48155249864794E-2</v>
       </c>
       <c r="DI24">
-        <f t="shared" si="0"/>
+        <f>CU24-CY24</f>
         <v>-1.8970003176945971E-2</v>
       </c>
     </row>
@@ -10048,7 +10057,7 @@
         <v>-1.4804399979766399E-2</v>
       </c>
       <c r="DB25" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC25">
         <v>4.6772684203460799E-2</v>
@@ -10069,7 +10078,7 @@
         <v>1.0777441784739401E-2</v>
       </c>
       <c r="DI25">
-        <f t="shared" si="0"/>
+        <f>CU25-CY25</f>
         <v>1.0874099971260986E-2</v>
       </c>
     </row>
@@ -10408,7 +10417,7 @@
         <v>-1.46294998703524E-2</v>
       </c>
       <c r="DB26" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC26">
         <v>1.5523249749094199E-2</v>
@@ -10429,7 +10438,7 @@
         <v>-3.9077547262422697E-3</v>
       </c>
       <c r="DI26">
-        <f t="shared" si="0"/>
+        <f>CU26-CY26</f>
         <v>-7.1765678003429811E-3</v>
       </c>
     </row>
@@ -10768,7 +10777,7 @@
         <v>-1.42141273390734E-2</v>
       </c>
       <c r="DB27" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC27">
         <v>1.8741021223831901E-2</v>
@@ -10789,7 +10798,7 @@
         <v>-2.38887080340646E-2</v>
       </c>
       <c r="DI27">
-        <f t="shared" si="0"/>
+        <f>CU27-CY27</f>
         <v>-2.665731867818899E-2</v>
       </c>
     </row>
@@ -11128,7 +11137,7 @@
         <v>-1.1908287357073199E-2</v>
       </c>
       <c r="DB28" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC28">
         <v>1.7411787179298699E-2</v>
@@ -11149,7 +11158,7 @@
         <v>5.4335498483851503E-2</v>
       </c>
       <c r="DI28">
-        <f t="shared" si="0"/>
+        <f>CU28-CY28</f>
         <v>-2.8225127607600653E-4</v>
       </c>
     </row>
@@ -11488,7 +11497,7 @@
         <v>-9.8830033093690803E-3</v>
       </c>
       <c r="DB29" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC29">
         <v>-5.2535999966494204E-3</v>
@@ -11509,7 +11518,7 @@
         <v>-3.0835699999443002E-2</v>
       </c>
       <c r="DI29">
-        <f t="shared" si="0"/>
+        <f>CU29-CY29</f>
         <v>-3.5533410264180221E-3</v>
       </c>
     </row>
@@ -11848,7 +11857,7 @@
         <v>-8.6400000072899205E-3</v>
       </c>
       <c r="DB30" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC30">
         <v>-1.97798926965333E-2</v>
@@ -11869,7 +11878,7 @@
         <v>-6.6810418211389298E-3</v>
       </c>
       <c r="DI30">
-        <f t="shared" si="0"/>
+        <f>CU30-CY30</f>
         <v>1.3752999948339895E-3</v>
       </c>
     </row>
@@ -12208,7 +12217,7 @@
         <v>-8.5677397437393596E-3</v>
       </c>
       <c r="DB31" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC31">
         <v>-8.03946796804666E-3</v>
@@ -12229,7 +12238,7 @@
         <v>1.5386138577014199E-2</v>
       </c>
       <c r="DI31">
-        <f t="shared" si="0"/>
+        <f>CU31-CY31</f>
         <v>-4.0404099272560168E-3</v>
       </c>
     </row>
@@ -12568,7 +12577,7 @@
         <v>-9.1619975864887205E-4</v>
       </c>
       <c r="DB32" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="DC32">
         <v>-1.49743710644543E-2</v>
@@ -12589,7 +12598,7 @@
         <v>-5.1001612097024897E-2</v>
       </c>
       <c r="DI32">
-        <f t="shared" si="0"/>
+        <f>CU32-CY32</f>
         <v>2.1195899695158005E-2</v>
       </c>
     </row>
@@ -12928,7 +12937,7 @@
         <v>4.36207861639559E-4</v>
       </c>
       <c r="DB33" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC33">
         <v>-3.5793193412246099E-2</v>
@@ -12949,7 +12958,7 @@
         <v>-8.1828969705384207E-3</v>
       </c>
       <c r="DI33">
-        <f t="shared" si="0"/>
+        <f>CU33-CY33</f>
         <v>-4.1779354796794843E-4</v>
       </c>
     </row>
@@ -13288,7 +13297,7 @@
         <v>1.46770582068711E-3</v>
       </c>
       <c r="DB34" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC34">
         <v>-4.4672297779470599E-2</v>
@@ -13309,7 +13318,7 @@
         <v>5.8311953194788602E-2</v>
       </c>
       <c r="DI34">
-        <f t="shared" si="0"/>
+        <f>CU34-CY34</f>
         <v>8.945549139752984E-3</v>
       </c>
     </row>
@@ -13648,7 +13657,7 @@
         <v>2.90569999197032E-3</v>
       </c>
       <c r="DB35" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC35">
         <v>-6.0921791708096799E-2</v>
@@ -13669,7 +13678,7 @@
         <v>2.0691849407739899E-2</v>
       </c>
       <c r="DI35">
-        <f t="shared" si="0"/>
+        <f>CU35-CY35</f>
         <v>-7.1944000083020154E-3</v>
       </c>
     </row>
@@ -14008,7 +14017,7 @@
         <v>3.5974316997453501E-3</v>
       </c>
       <c r="DB36" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC36">
         <v>3.12500000291038E-3</v>
@@ -14029,7 +14038,7 @@
         <v>-1.10023999877739E-2</v>
       </c>
       <c r="DI36">
-        <f t="shared" si="0"/>
+        <f>CU36-CY36</f>
         <v>-2.0272345282139614E-3</v>
       </c>
     </row>
@@ -14368,7 +14377,7 @@
         <v>3.8541569447261199E-3</v>
       </c>
       <c r="DB37" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC37">
         <v>2.0173534401692401E-2</v>
@@ -14389,7 +14398,7 @@
         <v>1.59071705711539E-2</v>
       </c>
       <c r="DI37">
-        <f t="shared" si="0"/>
+        <f>CU37-CY37</f>
         <v>-1.9277576793690354E-3</v>
       </c>
     </row>
@@ -14728,7 +14737,7 @@
         <v>4.8675428697606497E-3</v>
       </c>
       <c r="DB38" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC38">
         <v>-0.119005200045648</v>
@@ -14749,7 +14758,7 @@
         <v>1.45321000018157E-2</v>
       </c>
       <c r="DI38">
-        <f t="shared" si="0"/>
+        <f>CU38-CY38</f>
         <v>-6.1559346358989742E-3</v>
       </c>
     </row>
@@ -15088,7 +15097,7 @@
         <v>5.8379120018798797E-3</v>
       </c>
       <c r="DB39" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC39">
         <v>-1.63951474823988E-2</v>
@@ -15109,7 +15118,7 @@
         <v>-2.32713498990051E-2</v>
       </c>
       <c r="DI39">
-        <f t="shared" si="0"/>
+        <f>CU39-CY39</f>
         <v>2.2527536057169006E-2</v>
       </c>
     </row>
@@ -15448,7 +15457,7 @@
         <v>6.2309500062838197E-3</v>
       </c>
       <c r="DB40" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC40">
         <v>-1.3836700003594099E-2</v>
@@ -15469,7 +15478,7 @@
         <v>-8.4609999976237305E-3</v>
       </c>
       <c r="DI40">
-        <f t="shared" si="0"/>
+        <f>CU40-CY40</f>
         <v>-1.543111767387001E-2</v>
       </c>
     </row>
@@ -15808,7 +15817,7 @@
         <v>1.2136934150476E-2</v>
       </c>
       <c r="DB41" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC41">
         <v>-0.11602759995730499</v>
@@ -15829,7 +15838,7 @@
         <v>-9.1440399992279695E-2</v>
       </c>
       <c r="DI41">
-        <f t="shared" si="0"/>
+        <f>CU41-CY41</f>
         <v>1.2935537844896983E-2</v>
       </c>
     </row>
@@ -16168,7 +16177,7 @@
         <v>2.07562929717823E-2</v>
       </c>
       <c r="DB42" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="DC42">
         <v>-0.18023115000687501</v>
@@ -16189,7 +16198,7 @@
         <v>1.03698999155312E-2</v>
       </c>
       <c r="DI42">
-        <f t="shared" si="0"/>
+        <f>CU42-CY42</f>
         <v>4.0549613069743029E-2</v>
       </c>
     </row>
@@ -16528,7 +16537,7 @@
         <v>3.5044225828187302E-2</v>
       </c>
       <c r="DB43" t="s">
-        <v>64</v>
+        <v>207</v>
       </c>
       <c r="DC43">
         <v>-5.0415999721735699E-3</v>
@@ -16549,7 +16558,7 @@
         <v>-9.8269999725744094E-3</v>
       </c>
       <c r="DI43">
-        <f t="shared" si="0"/>
+        <f>CU43-CY43</f>
         <v>3.1233236636579731E-3</v>
       </c>
     </row>
@@ -16888,7 +16897,7 @@
         <v>5.40236873202957E-2</v>
       </c>
       <c r="DB44" t="s">
-        <v>64</v>
+        <v>207</v>
       </c>
       <c r="DC44">
         <v>-8.8969799922779202E-2</v>
@@ -16909,7 +16918,7 @@
         <v>-6.0773400124162401E-2</v>
       </c>
       <c r="DI44">
-        <f t="shared" si="0"/>
+        <f>CU44-CY44</f>
         <v>6.8547371934983004E-2</v>
       </c>
     </row>
@@ -17248,7 +17257,7 @@
         <v>6.4827359397895606E-2</v>
       </c>
       <c r="DB45" t="s">
-        <v>64</v>
+        <v>207</v>
       </c>
       <c r="DC45">
         <v>-1.5547099988907499E-2</v>
@@ -17269,7 +17278,7 @@
         <v>-0.10414369998034</v>
       </c>
       <c r="DI45">
-        <f t="shared" si="0"/>
+        <f>CU45-CY45</f>
         <v>1.1723811156117037E-2</v>
       </c>
     </row>
@@ -17608,7 +17617,7 @@
         <v>7.3251906142104403E-2</v>
       </c>
       <c r="DB46" t="s">
-        <v>64</v>
+        <v>207</v>
       </c>
       <c r="DC46">
         <v>-2.7425399515777799E-2</v>
@@ -17629,7 +17638,7 @@
         <v>-2.4841600097715799E-2</v>
       </c>
       <c r="DI46">
-        <f t="shared" si="0"/>
+        <f>CU46-CY46</f>
         <v>8.0505915102548953E-2</v>
       </c>
     </row>
@@ -17968,7 +17977,7 @@
         <v>7.6968276669504093E-2</v>
       </c>
       <c r="DB47" t="s">
-        <v>64</v>
+        <v>207</v>
       </c>
       <c r="DC47">
         <v>7.7434499748051097E-2</v>
@@ -17989,12 +17998,12 @@
         <v>-0.10168130020610899</v>
       </c>
       <c r="DI47">
-        <f t="shared" si="0"/>
+        <f>CU47-CY47</f>
         <v>4.2992998933186977E-2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DA47">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DI47">
     <sortCondition ref="DA1:DA47"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
update plot for fig 4
</commit_message>
<xml_diff>
--- a/code/total_df_n46.xlsx
+++ b/code/total_df_n46.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-mid-clean/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9555B970-7F64-5642-8BE5-0DAC00F74835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D07BD14-A6A7-3A47-8C6B-2D0EDA1CC9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="1220" windowWidth="19600" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="208">
   <si>
     <t>Sub</t>
   </si>
@@ -653,13 +653,13 @@
     <t>LG_N_split</t>
   </si>
   <si>
-    <t>Avg</t>
-  </si>
-  <si>
-    <t>Low (-1SD)</t>
-  </si>
-  <si>
-    <t>High (+1SD)</t>
+    <t>LG_N_perc</t>
+  </si>
+  <si>
+    <t>LG_N_splitthree</t>
+  </si>
+  <si>
+    <t>Med</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -695,6 +695,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -746,6 +752,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,13 +1087,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DI47"/>
+  <dimension ref="A1:DK47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CW21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DC58" sqref="DC58"/>
+      <selection pane="bottomRight" activeCell="DF23" sqref="DF23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1101,7 +1108,7 @@
     <col min="94" max="96" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" ht="42" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:115" ht="42" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1411,38 +1418,44 @@
       <c r="CY1" t="s">
         <v>194</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="CZ1" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DA1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DB1" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DC1" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="DD1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DG1" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DI1" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" s="11" t="s">
         <v>203</v>
       </c>
+      <c r="DK1" t="s">
+        <v>205</v>
+      </c>
     </row>
-    <row r="2" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1777,32 +1790,39 @@
         <v>-0.25457835011184199</v>
       </c>
       <c r="DB2" t="s">
-        <v>206</v>
-      </c>
-      <c r="DC2">
+        <v>154</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD2">
         <v>-1.16798956878483E-2</v>
       </c>
-      <c r="DD2">
+      <c r="DE2">
         <v>-2.38157697021961E-2</v>
       </c>
-      <c r="DE2">
+      <c r="DF2">
         <v>3.0062717036344101E-2</v>
       </c>
-      <c r="DF2">
+      <c r="DG2">
         <v>-2.9366146191023199E-3</v>
       </c>
-      <c r="DG2">
+      <c r="DH2">
         <v>-1.50724886334501E-2</v>
       </c>
-      <c r="DH2">
+      <c r="DI2">
         <v>-5.3878486738540197E-2</v>
       </c>
-      <c r="DI2">
+      <c r="DJ2">
         <f>CU2-CY2</f>
         <v>-7.2201899951323034E-2</v>
       </c>
+      <c r="DK2">
+        <f>((CW2-CU2)/CU2)*100</f>
+        <v>99.732528855451292</v>
+      </c>
     </row>
-    <row r="3" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2137,32 +2157,39 @@
         <v>-0.14633959997445301</v>
       </c>
       <c r="DB3" t="s">
-        <v>206</v>
-      </c>
-      <c r="DC3">
+        <v>154</v>
+      </c>
+      <c r="DC3" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD3">
         <v>2.09843575867125E-2</v>
       </c>
-      <c r="DD3">
+      <c r="DE3">
         <v>-1.4523684614687201E-2</v>
       </c>
-      <c r="DE3">
+      <c r="DF3">
         <v>6.6652066103415494E-2</v>
       </c>
-      <c r="DF3">
+      <c r="DG3">
         <v>6.8547371934982906E-2</v>
       </c>
-      <c r="DG3">
+      <c r="DH3">
         <v>3.3039329733583103E-2</v>
       </c>
-      <c r="DH3">
+      <c r="DI3">
         <v>-8.1175750718102693E-2</v>
       </c>
-      <c r="DI3">
+      <c r="DJ3">
         <f>CU3-CY3</f>
         <v>-6.7212299967649991E-2</v>
       </c>
+      <c r="DK3">
+        <f>((CW3-CU3)/CU3)*100</f>
+        <v>53.256172193528037</v>
+      </c>
     </row>
-    <row r="4" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -2497,32 +2524,39 @@
         <v>-0.13521959981880999</v>
       </c>
       <c r="DB4" t="s">
-        <v>206</v>
-      </c>
-      <c r="DC4">
+        <v>154</v>
+      </c>
+      <c r="DC4" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD4">
         <v>1.6252809669822399E-2</v>
       </c>
-      <c r="DD4">
+      <c r="DE4">
         <v>-1.97933200979605E-2</v>
       </c>
-      <c r="DE4">
+      <c r="DF4">
         <v>2.0062439260072999E-2</v>
       </c>
-      <c r="DF4">
+      <c r="DG4">
         <v>4.0549613069742897E-2</v>
       </c>
-      <c r="DG4">
+      <c r="DH4">
         <v>4.5034833019599301E-3</v>
       </c>
-      <c r="DH4">
+      <c r="DI4">
         <v>-3.9855759358033503E-2</v>
       </c>
-      <c r="DI4">
+      <c r="DJ4">
         <f>CU4-CY4</f>
         <v>-1.7357699805869986E-2</v>
       </c>
+      <c r="DK4">
+        <f>((CW4-CU4)/CU4)*100</f>
+        <v>43.738575620087964</v>
+      </c>
     </row>
-    <row r="5" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -2857,32 +2891,39 @@
         <v>-0.10734460002277001</v>
       </c>
       <c r="DB5" t="s">
-        <v>206</v>
-      </c>
-      <c r="DC5">
+        <v>154</v>
+      </c>
+      <c r="DC5" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD5">
         <v>-1.6335683467332201E-2</v>
       </c>
-      <c r="DD5">
+      <c r="DE5">
         <v>-2.2995747160166499E-2</v>
       </c>
-      <c r="DE5">
+      <c r="DF5">
         <v>-2.3085704888217099E-3</v>
       </c>
-      <c r="DF5">
+      <c r="DG5">
         <v>-4.0481117321178301E-4</v>
       </c>
-      <c r="DG5">
+      <c r="DH5">
         <v>-7.0648748660460097E-3</v>
       </c>
-      <c r="DH5">
+      <c r="DI5">
         <v>-2.06871766713447E-2</v>
       </c>
-      <c r="DI5">
+      <c r="DJ5">
         <f>CU5-CY5</f>
         <v>-1.2593000021297984E-2</v>
       </c>
+      <c r="DK5">
+        <f>((CW5-CU5)/CU5)*100</f>
+        <v>41.236947868391312</v>
+      </c>
     </row>
-    <row r="6" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -3217,32 +3258,39 @@
         <v>-6.3504914636723697E-2</v>
       </c>
       <c r="DB6" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC6">
+        <v>154</v>
+      </c>
+      <c r="DC6" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD6">
         <v>-7.8944207634776796E-3</v>
       </c>
-      <c r="DD6">
+      <c r="DE6">
         <v>-7.4529320700094104E-3</v>
       </c>
-      <c r="DE6">
+      <c r="DF6">
         <v>-1.2773134279996099E-2</v>
       </c>
-      <c r="DF6">
+      <c r="DG6">
         <v>-7.1765678003430297E-3</v>
       </c>
-      <c r="DG6">
+      <c r="DH6">
         <v>-6.7350791068747596E-3</v>
       </c>
-      <c r="DH6">
+      <c r="DI6">
         <v>5.3202022099867402E-3</v>
       </c>
-      <c r="DI6">
+      <c r="DJ6">
         <f>CU6-CY6</f>
         <v>-2.2397127133444994E-2</v>
       </c>
+      <c r="DK6">
+        <f>((CW6-CU6)/CU6)*100</f>
+        <v>24.836485561660268</v>
+      </c>
     </row>
-    <row r="7" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -3577,32 +3625,39 @@
         <v>-5.5414395945262998E-2</v>
       </c>
       <c r="DB7" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC7">
+        <v>154</v>
+      </c>
+      <c r="DC7" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD7">
         <v>1.55828368733637E-2</v>
       </c>
-      <c r="DD7">
+      <c r="DE7">
         <v>4.0047986549325201E-3</v>
       </c>
-      <c r="DE7">
+      <c r="DF7">
         <v>2.2725756571162398E-2</v>
       </c>
-      <c r="DF7">
+      <c r="DG7">
         <v>-1.8970003176946099E-2</v>
       </c>
-      <c r="DG7">
+      <c r="DH7">
         <v>-3.0548041395377298E-2</v>
       </c>
-      <c r="DH7">
+      <c r="DI7">
         <v>-1.8720957916229901E-2</v>
       </c>
-      <c r="DI7">
+      <c r="DJ7">
         <f>CU7-CY7</f>
         <v>1.0023120528786011E-2</v>
       </c>
+      <c r="DK7">
+        <f>((CW7-CU7)/CU7)*100</f>
+        <v>18.763594733807405</v>
+      </c>
     </row>
-    <row r="8" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -3937,32 +3992,39 @@
         <v>-5.11482999427244E-2</v>
       </c>
       <c r="DB8" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC8">
+        <v>154</v>
+      </c>
+      <c r="DC8" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD8">
         <v>-1.18083389243111E-2</v>
       </c>
-      <c r="DD8">
+      <c r="DE8">
         <v>-2.3506192490458402E-2</v>
       </c>
-      <c r="DE8">
+      <c r="DF8">
         <v>-1.8524544779211199E-2</v>
       </c>
-      <c r="DF8">
+      <c r="DG8">
         <v>-1.8702045723330198E-2</v>
       </c>
-      <c r="DG8">
+      <c r="DH8">
         <v>-3.0399899289477599E-2</v>
       </c>
-      <c r="DH8">
+      <c r="DI8">
         <v>-4.9816477112471997E-3</v>
       </c>
-      <c r="DI8">
+      <c r="DJ8">
         <f>CU8-CY8</f>
         <v>-3.0303999083109989E-3</v>
       </c>
+      <c r="DK8">
+        <f>((CW8-CU8)/CU8)*100</f>
+        <v>19.278612893396073</v>
+      </c>
     </row>
-    <row r="9" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -4297,32 +4359,39 @@
         <v>-5.08987195789814E-2</v>
       </c>
       <c r="DB9" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC9">
+        <v>154</v>
+      </c>
+      <c r="DC9" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD9">
         <v>-5.0698698614723897E-2</v>
       </c>
-      <c r="DD9">
+      <c r="DE9">
         <v>-5.9955008910037501E-2</v>
       </c>
-      <c r="DE9">
+      <c r="DF9">
         <v>-3.0194626073352899E-2</v>
       </c>
-      <c r="DF9">
+      <c r="DG9">
         <v>3.7174064782448099E-2</v>
       </c>
-      <c r="DG9">
+      <c r="DH9">
         <v>2.7917754487134499E-2</v>
       </c>
-      <c r="DH9">
+      <c r="DI9">
         <v>-2.9760382836684501E-2</v>
       </c>
-      <c r="DI9">
+      <c r="DJ9">
         <f>CU9-CY9</f>
         <v>-4.1412376682273988E-2</v>
       </c>
+      <c r="DK9">
+        <f>((CW9-CU9)/CU9)*100</f>
+        <v>18.784787637166882</v>
+      </c>
     </row>
-    <row r="10" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -4657,32 +4726,39 @@
         <v>-4.3319212622009197E-2</v>
       </c>
       <c r="DB10" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC10">
+        <v>154</v>
+      </c>
+      <c r="DC10" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD10">
         <v>-1.1424083008023399E-2</v>
       </c>
-      <c r="DD10">
+      <c r="DE10">
         <v>-1.8792350899275299E-2</v>
       </c>
-      <c r="DE10">
+      <c r="DF10">
         <v>1.1270429635260299E-2</v>
       </c>
-      <c r="DF10">
+      <c r="DG10">
         <v>1.7301852794844299E-3</v>
       </c>
-      <c r="DG10">
+      <c r="DH10">
         <v>-5.6380826117674501E-3</v>
       </c>
-      <c r="DH10">
+      <c r="DI10">
         <v>-3.0062780534535701E-2</v>
       </c>
-      <c r="DI10">
+      <c r="DJ10">
         <f>CU10-CY10</f>
         <v>-1.6260741744189983E-2</v>
       </c>
+      <c r="DK10">
+        <f>((CW10-CU10)/CU10)*100</f>
+        <v>20.381725008073957</v>
+      </c>
     </row>
-    <row r="11" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -5017,32 +5093,39 @@
         <v>-4.2208238213788697E-2</v>
       </c>
       <c r="DB11" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC11">
+        <v>154</v>
+      </c>
+      <c r="DC11" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD11">
         <v>2.6066434336826198E-2</v>
       </c>
-      <c r="DD11">
+      <c r="DE11">
         <v>-1.1626036080997401E-2</v>
       </c>
-      <c r="DE11">
+      <c r="DF11">
         <v>3.6354418203700299E-2</v>
       </c>
-      <c r="DF11">
+      <c r="DG11">
         <v>-2.8225127607584E-4</v>
       </c>
-      <c r="DG11">
+      <c r="DH11">
         <v>-3.7974721693899399E-2</v>
       </c>
-      <c r="DH11">
+      <c r="DI11">
         <v>-4.7980454284697702E-2</v>
       </c>
-      <c r="DI11">
+      <c r="DJ11">
         <f>CU11-CY11</f>
         <v>-1.8702045723331007E-2</v>
       </c>
+      <c r="DK11">
+        <f>((CW11-CU11)/CU11)*100</f>
+        <v>16.218164588342926</v>
+      </c>
     </row>
-    <row r="12" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -5377,32 +5460,39 @@
         <v>-3.5077569467830402E-2</v>
       </c>
       <c r="DB12" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC12">
+        <v>154</v>
+      </c>
+      <c r="DC12" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD12">
         <v>-8.8674982544034698E-4</v>
       </c>
-      <c r="DD12">
+      <c r="DE12">
         <v>-4.5273298164829603E-3</v>
       </c>
-      <c r="DE12">
+      <c r="DF12">
         <v>9.4757729675620697E-4</v>
       </c>
-      <c r="DF12">
+      <c r="DG12">
         <v>-4.0404099272564001E-3</v>
       </c>
-      <c r="DG12">
+      <c r="DH12">
         <v>-7.6809899182990098E-3</v>
       </c>
-      <c r="DH12">
+      <c r="DI12">
         <v>-5.4749071132391596E-3</v>
       </c>
-      <c r="DI12">
+      <c r="DJ12">
         <f>CU12-CY12</f>
         <v>-4.6165993087925017E-2</v>
       </c>
+      <c r="DK12">
+        <f>((CW12-CU12)/CU12)*100</f>
+        <v>12.015469211177084</v>
+      </c>
     </row>
-    <row r="13" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>54</v>
       </c>
@@ -5737,32 +5827,39 @@
         <v>-3.2821400000102502E-2</v>
       </c>
       <c r="DB13" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC13">
+        <v>154</v>
+      </c>
+      <c r="DC13" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD13">
         <v>2.9919088934548199E-2</v>
       </c>
-      <c r="DD13">
+      <c r="DE13">
         <v>-1.6865344427060301E-2</v>
       </c>
-      <c r="DE13">
+      <c r="DF13">
         <v>1.5005051856860499E-2</v>
       </c>
-      <c r="DF13">
+      <c r="DG13">
         <v>-6.4615916926413699E-4</v>
       </c>
-      <c r="DG13">
+      <c r="DH13">
         <v>-4.7430592530872603E-2</v>
       </c>
-      <c r="DH13">
+      <c r="DI13">
         <v>-3.1870396283920799E-2</v>
       </c>
-      <c r="DI13">
+      <c r="DJ13">
         <f>CU13-CY13</f>
         <v>-1.7598600003112003E-2</v>
       </c>
+      <c r="DK13">
+        <f>((CW13-CU13)/CU13)*100</f>
+        <v>13.650574343681157</v>
+      </c>
     </row>
-    <row r="14" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -6097,32 +6194,39 @@
         <v>-2.7202937097172201E-2</v>
       </c>
       <c r="DB14" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC14">
+        <v>154</v>
+      </c>
+      <c r="DC14" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD14">
         <v>4.2111438873689601E-2</v>
       </c>
-      <c r="DD14">
+      <c r="DE14">
         <v>-7.2540089604444802E-3</v>
       </c>
-      <c r="DE14">
+      <c r="DF14">
         <v>8.4970466210506801E-2</v>
       </c>
-      <c r="DF14">
+      <c r="DG14">
         <v>8.0505915102548897E-2</v>
       </c>
-      <c r="DG14">
+      <c r="DH14">
         <v>3.1140467268414702E-2</v>
       </c>
-      <c r="DH14">
+      <c r="DI14">
         <v>-9.2224475170951295E-2</v>
       </c>
-      <c r="DI14">
+      <c r="DJ14">
         <f>CU14-CY14</f>
         <v>-7.6408453987829861E-3</v>
       </c>
+      <c r="DK14">
+        <f>((CW14-CU14)/CU14)*100</f>
+        <v>11.501849454453767</v>
+      </c>
     </row>
-    <row r="15" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -6457,32 +6561,39 @@
         <v>-2.6762782828882298E-2</v>
       </c>
       <c r="DB15" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC15">
+        <v>154</v>
+      </c>
+      <c r="DC15" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD15">
         <v>-3.5798626782707198E-2</v>
       </c>
-      <c r="DD15">
+      <c r="DE15">
         <v>1.24431913391163E-2</v>
       </c>
-      <c r="DE15">
+      <c r="DF15">
         <v>5.5574758011061903E-2</v>
       </c>
-      <c r="DF15">
+      <c r="DG15">
         <v>-2.6657318678189702E-2</v>
       </c>
-      <c r="DG15">
+      <c r="DH15">
         <v>2.15844994436338E-2</v>
       </c>
-      <c r="DH15">
+      <c r="DI15">
         <v>-4.31315666719456E-2</v>
       </c>
-      <c r="DI15">
+      <c r="DJ15">
         <f>CU15-CY15</f>
         <v>8.494502911344104E-2</v>
       </c>
+      <c r="DK15">
+        <f>((CW15-CU15)/CU15)*100</f>
+        <v>6.5666344357256756</v>
+      </c>
     </row>
-    <row r="16" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
@@ -6817,32 +6928,39 @@
         <v>-2.6752384321298402E-2</v>
       </c>
       <c r="DB16" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC16">
+        <v>154</v>
+      </c>
+      <c r="DC16" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD16">
         <v>6.2691368275409297E-3</v>
       </c>
-      <c r="DD16">
+      <c r="DE16">
         <v>-6.4322989082938797E-3</v>
       </c>
-      <c r="DE16">
+      <c r="DF16">
         <v>-2.01993445152766E-2</v>
       </c>
-      <c r="DF16">
+      <c r="DG16">
         <v>-1.2112331582102299E-2</v>
       </c>
-      <c r="DG16">
+      <c r="DH16">
         <v>-2.4813767317937101E-2</v>
       </c>
-      <c r="DH16">
+      <c r="DI16">
         <v>1.3767045606982701E-2</v>
       </c>
-      <c r="DI16">
+      <c r="DJ16">
         <f>CU16-CY16</f>
         <v>-2.9366146191029951E-3</v>
       </c>
+      <c r="DK16">
+        <f>((CW16-CU16)/CU16)*100</f>
+        <v>8.7587918713223321</v>
+      </c>
     </row>
-    <row r="17" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -7177,32 +7295,39 @@
         <v>-2.3400558333378198E-2</v>
       </c>
       <c r="DB17" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC17">
+        <v>154</v>
+      </c>
+      <c r="DC17" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD17">
         <v>-3.4930104171507902E-2</v>
       </c>
-      <c r="DD17">
+      <c r="DE17">
         <v>1.10884236200945E-2</v>
       </c>
-      <c r="DE17">
+      <c r="DF17">
         <v>-3.0989143429906101E-2</v>
       </c>
-      <c r="DF17">
+      <c r="DG17">
         <v>-4.6165993087925003E-2</v>
       </c>
-      <c r="DG17">
+      <c r="DH17">
         <v>-1.47465296322479E-4</v>
       </c>
-      <c r="DH17">
+      <c r="DI17">
         <v>4.2077567050000597E-2</v>
       </c>
-      <c r="DI17">
+      <c r="DJ17">
         <f>CU17-CY17</f>
         <v>-4.0481117321200522E-4</v>
       </c>
+      <c r="DK17">
+        <f>((CW17-CU17)/CU17)*100</f>
+        <v>8.6200598342233405</v>
+      </c>
     </row>
-    <row r="18" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
@@ -7537,32 +7662,39 @@
         <v>-2.2780944127589398E-2</v>
       </c>
       <c r="DB18" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC18">
+        <v>154</v>
+      </c>
+      <c r="DC18" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD18">
         <v>-2.83212094800546E-2</v>
       </c>
-      <c r="DD18">
+      <c r="DE18">
         <v>-2.7058470877818701E-2</v>
       </c>
-      <c r="DE18">
+      <c r="DF18">
         <v>-4.5705526135861797E-2</v>
       </c>
-      <c r="DF18">
+      <c r="DG18">
         <v>-1.6260741744190399E-2</v>
       </c>
-      <c r="DG18">
+      <c r="DH18">
         <v>-1.49980031419545E-2</v>
       </c>
-      <c r="DH18">
+      <c r="DI18">
         <v>1.86470552580431E-2</v>
       </c>
-      <c r="DI18">
+      <c r="DJ18">
         <f>CU18-CY18</f>
         <v>3.7174064782448002E-2</v>
       </c>
+      <c r="DK18">
+        <f>((CW18-CU18)/CU18)*100</f>
+        <v>6.7329983954492159</v>
+      </c>
     </row>
-    <row r="19" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -7897,32 +8029,39 @@
         <v>-1.9896449986845199E-2</v>
       </c>
       <c r="DB19" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC19">
+        <v>154</v>
+      </c>
+      <c r="DC19" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD19">
         <v>-1.2799153337255099E-2</v>
       </c>
-      <c r="DD19">
+      <c r="DE19">
         <v>5.6246662279590904E-3</v>
       </c>
-      <c r="DE19">
+      <c r="DF19">
         <v>2.3734838468953902E-3</v>
       </c>
-      <c r="DF19">
+      <c r="DG19">
         <v>-2.0272345282137299E-3</v>
       </c>
-      <c r="DG19">
+      <c r="DH19">
         <v>1.6396585037000401E-2</v>
       </c>
-      <c r="DH19">
+      <c r="DI19">
         <v>3.2511823810636902E-3</v>
       </c>
-      <c r="DI19">
+      <c r="DJ19">
         <f>CU19-CY19</f>
         <v>6.3898500520739865E-3</v>
       </c>
+      <c r="DK19">
+        <f>((CW19-CU19)/CU19)*100</f>
+        <v>5.6269919779363349</v>
+      </c>
     </row>
-    <row r="20" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -8257,32 +8396,39 @@
         <v>-1.8544630490396199E-2</v>
       </c>
       <c r="DB20" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC20">
+        <v>154</v>
+      </c>
+      <c r="DC20" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD20">
         <v>-2.4216965413870601E-2</v>
       </c>
-      <c r="DD20">
+      <c r="DE20">
         <v>-1.9562091698389801E-2</v>
       </c>
-      <c r="DE20">
+      <c r="DF20">
         <v>-8.7017762489267608E-3</v>
       </c>
-      <c r="DF20">
+      <c r="DG20">
         <v>-7.6408453987823997E-3</v>
       </c>
-      <c r="DG20">
+      <c r="DH20">
         <v>-2.9859716833016102E-3</v>
       </c>
-      <c r="DH20">
+      <c r="DI20">
         <v>-1.0860315449463E-2</v>
       </c>
-      <c r="DI20">
+      <c r="DJ20">
         <f>CU20-CY20</f>
         <v>-1.2112331582102009E-2</v>
       </c>
+      <c r="DK20">
+        <f>((CW20-CU20)/CU20)*100</f>
+        <v>6.8763341150044566</v>
+      </c>
     </row>
-    <row r="21" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -8617,32 +8763,39 @@
         <v>-1.7731455503962899E-2</v>
       </c>
       <c r="DB21" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC21">
+        <v>154</v>
+      </c>
+      <c r="DC21" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD21">
         <v>8.0859563677222399E-3</v>
       </c>
-      <c r="DD21">
+      <c r="DE21">
         <v>5.7819146240944896E-3</v>
       </c>
-      <c r="DE21">
+      <c r="DF21">
         <v>-5.3491804428631396E-3</v>
       </c>
-      <c r="DF21">
+      <c r="DG21">
         <v>-1.92775767936836E-3</v>
       </c>
-      <c r="DG21">
+      <c r="DH21">
         <v>-4.23179942299611E-3</v>
       </c>
-      <c r="DH21">
+      <c r="DI21">
         <v>1.11310950669576E-2</v>
       </c>
-      <c r="DI21">
+      <c r="DJ21">
         <f>CU21-CY21</f>
         <v>-3.2554207427893E-2</v>
       </c>
+      <c r="DK21">
+        <f>((CW21-CU21)/CU21)*100</f>
+        <v>5.0216637954362504</v>
+      </c>
     </row>
-    <row r="22" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -8977,32 +9130,39 @@
         <v>-1.7511503596324401E-2</v>
       </c>
       <c r="DB22" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC22">
+        <v>154</v>
+      </c>
+      <c r="DC22" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD22">
         <v>8.2142521860077908E-3</v>
       </c>
-      <c r="DD22">
+      <c r="DE22">
         <v>2.1662067680153899E-2</v>
       </c>
-      <c r="DE22">
+      <c r="DF22">
         <v>7.5217568082734899E-3</v>
       </c>
-      <c r="DF22">
+      <c r="DG22">
         <v>-1.54311176738701E-2</v>
       </c>
-      <c r="DG22">
+      <c r="DH22">
         <v>-1.9833021797239698E-3</v>
       </c>
-      <c r="DH22">
+      <c r="DI22">
         <v>1.41403108718805E-2</v>
       </c>
-      <c r="DI22">
+      <c r="DJ22">
         <f>CU22-CY22</f>
         <v>-6.4615916926402672E-4</v>
       </c>
+      <c r="DK22">
+        <f>((CW22-CU22)/CU22)*100</f>
+        <v>5.8697255634242431</v>
+      </c>
     </row>
-    <row r="23" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
@@ -9337,32 +9497,39 @@
         <v>-1.70621656197909E-2</v>
       </c>
       <c r="DB23" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC23">
+        <v>154</v>
+      </c>
+      <c r="DC23" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD23">
         <v>9.6614288777345791E-3</v>
       </c>
-      <c r="DD23">
+      <c r="DE23">
         <v>3.1920902164529197E-2</v>
       </c>
-      <c r="DE23">
+      <c r="DF23">
         <v>3.5264441805338699E-2</v>
       </c>
-      <c r="DF23">
+      <c r="DG23">
         <v>3.1233236636580802E-3</v>
       </c>
-      <c r="DG23">
+      <c r="DH23">
         <v>2.5382796950452698E-2</v>
       </c>
-      <c r="DH23">
+      <c r="DI23">
         <v>-3.3435396408094602E-3</v>
       </c>
-      <c r="DI23">
+      <c r="DJ23">
         <f>CU23-CY23</f>
         <v>1.7301852794839867E-3</v>
       </c>
+      <c r="DK23">
+        <f>((CW23-CU23)/CU23)*100</f>
+        <v>6.3084606325579706</v>
+      </c>
     </row>
-    <row r="24" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -9697,32 +9864,39 @@
         <v>-1.49652045220136E-2</v>
       </c>
       <c r="DB24" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC24">
+        <v>154</v>
+      </c>
+      <c r="DC24" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD24">
         <v>1.9478247559163699E-2</v>
       </c>
-      <c r="DD24">
+      <c r="DE24">
         <v>3.3975277736317297E-2</v>
       </c>
-      <c r="DE24">
+      <c r="DF24">
         <v>9.1597527498379298E-3</v>
       </c>
-      <c r="DF24">
+      <c r="DG24">
         <v>4.2992998933186699E-2</v>
       </c>
-      <c r="DG24">
+      <c r="DH24">
         <v>5.7490029110340402E-2</v>
       </c>
-      <c r="DH24">
+      <c r="DI24">
         <v>2.48155249864794E-2</v>
       </c>
-      <c r="DI24">
+      <c r="DJ24">
         <f>CU24-CY24</f>
         <v>-1.8970003176945971E-2</v>
       </c>
+      <c r="DK24">
+        <f>((CW24-CU24)/CU24)*100</f>
+        <v>5.3386625062221613</v>
+      </c>
     </row>
-    <row r="25" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -10057,32 +10231,39 @@
         <v>-1.4804399979766399E-2</v>
       </c>
       <c r="DB25" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC25">
+        <v>155</v>
+      </c>
+      <c r="DC25" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD25">
         <v>4.6772684203460799E-2</v>
       </c>
-      <c r="DD25">
+      <c r="DE25">
         <v>5.3103548241779201E-2</v>
       </c>
-      <c r="DE25">
+      <c r="DF25">
         <v>4.23261064570397E-2</v>
       </c>
-      <c r="DF25">
+      <c r="DG25">
         <v>1.17238111561164E-2</v>
       </c>
-      <c r="DG25">
+      <c r="DH25">
         <v>1.8054675194434801E-2</v>
       </c>
-      <c r="DH25">
+      <c r="DI25">
         <v>1.0777441784739401E-2</v>
       </c>
-      <c r="DI25">
+      <c r="DJ25">
         <f>CU25-CY25</f>
         <v>1.0874099971260986E-2</v>
       </c>
+      <c r="DK25">
+        <f>((CW25-CU25)/CU25)*100</f>
+        <v>5.8825609588021823</v>
+      </c>
     </row>
-    <row r="26" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
@@ -10417,32 +10598,39 @@
         <v>-1.46294998703524E-2</v>
       </c>
       <c r="DB26" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC26">
+        <v>155</v>
+      </c>
+      <c r="DC26" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD26">
         <v>1.5523249749094199E-2</v>
       </c>
-      <c r="DD26">
+      <c r="DE26">
         <v>1.48227519239299E-2</v>
       </c>
-      <c r="DE26">
+      <c r="DF26">
         <v>1.8730506650172101E-2</v>
       </c>
-      <c r="DF26">
+      <c r="DG26">
         <v>-3.2554207427892799E-2</v>
       </c>
-      <c r="DG26">
+      <c r="DH26">
         <v>-3.3254705253057099E-2</v>
       </c>
-      <c r="DH26">
+      <c r="DI26">
         <v>-3.9077547262422697E-3</v>
       </c>
-      <c r="DI26">
+      <c r="DJ26">
         <f>CU26-CY26</f>
         <v>-7.1765678003429811E-3</v>
       </c>
+      <c r="DK26">
+        <f>((CW26-CU26)/CU26)*100</f>
+        <v>5.4116512599106885</v>
+      </c>
     </row>
-    <row r="27" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -10777,32 +10965,39 @@
         <v>-1.42141273390734E-2</v>
       </c>
       <c r="DB27" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC27">
+        <v>155</v>
+      </c>
+      <c r="DC27" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD27">
         <v>1.8741021223831901E-2</v>
       </c>
-      <c r="DD27">
+      <c r="DE27">
         <v>-7.4778433190658602E-3</v>
       </c>
-      <c r="DE27">
+      <c r="DF27">
         <v>1.64108647149987E-2</v>
       </c>
-      <c r="DF27">
+      <c r="DG27">
         <v>8.9455491397529806E-3</v>
       </c>
-      <c r="DG27">
+      <c r="DH27">
         <v>-1.72733154031448E-2</v>
       </c>
-      <c r="DH27">
+      <c r="DI27">
         <v>-2.38887080340646E-2</v>
       </c>
-      <c r="DI27">
+      <c r="DJ27">
         <f>CU27-CY27</f>
         <v>-2.665731867818899E-2</v>
       </c>
+      <c r="DK27">
+        <f>((CW27-CU27)/CU27)*100</f>
+        <v>5.0976932009146187</v>
+      </c>
     </row>
-    <row r="28" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -11137,32 +11332,39 @@
         <v>-1.1908287357073199E-2</v>
       </c>
       <c r="DB28" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC28">
+        <v>155</v>
+      </c>
+      <c r="DC28" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD28">
         <v>1.7411787179298699E-2</v>
       </c>
-      <c r="DD28">
+      <c r="DE28">
         <v>8.5400140960700799E-4</v>
       </c>
-      <c r="DE28">
+      <c r="DF28">
         <v>-5.3481497074244502E-2</v>
       </c>
-      <c r="DF28">
+      <c r="DG28">
         <v>-4.1779354796744802E-4</v>
       </c>
-      <c r="DG28">
+      <c r="DH28">
         <v>-1.6975579317659101E-2</v>
       </c>
-      <c r="DH28">
+      <c r="DI28">
         <v>5.4335498483851503E-2</v>
       </c>
-      <c r="DI28">
+      <c r="DJ28">
         <f>CU28-CY28</f>
         <v>-2.8225127607600653E-4</v>
       </c>
+      <c r="DK28">
+        <f>((CW28-CU28)/CU28)*100</f>
+        <v>4.1814779245239455</v>
+      </c>
     </row>
-    <row r="29" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -11497,32 +11699,39 @@
         <v>-9.8830033093690803E-3</v>
       </c>
       <c r="DB29" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC29">
+        <v>155</v>
+      </c>
+      <c r="DC29" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD29">
         <v>-5.2535999966494204E-3</v>
       </c>
-      <c r="DD29">
+      <c r="DE29">
         <v>-1.52227999969909E-2</v>
       </c>
-      <c r="DE29">
+      <c r="DF29">
         <v>1.5612900002451999E-2</v>
       </c>
-      <c r="DF29">
+      <c r="DG29">
         <v>-1.75986000031116E-2</v>
       </c>
-      <c r="DG29">
+      <c r="DH29">
         <v>-2.7567800003453099E-2</v>
       </c>
-      <c r="DH29">
+      <c r="DI29">
         <v>-3.0835699999443002E-2</v>
       </c>
-      <c r="DI29">
+      <c r="DJ29">
         <f>CU29-CY29</f>
         <v>-3.5533410264180221E-3</v>
       </c>
+      <c r="DK29">
+        <f>((CW29-CU29)/CU29)*100</f>
+        <v>3.9597529863957632</v>
+      </c>
     </row>
-    <row r="30" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -11857,32 +12066,39 @@
         <v>-8.6400000072899205E-3</v>
       </c>
       <c r="DB30" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC30">
+        <v>155</v>
+      </c>
+      <c r="DC30" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD30">
         <v>-1.97798926965333E-2</v>
       </c>
-      <c r="DD30">
+      <c r="DE30">
         <v>-1.6689624055288701E-2</v>
       </c>
-      <c r="DE30">
+      <c r="DF30">
         <v>-1.00085822341497E-2</v>
       </c>
-      <c r="DF30">
+      <c r="DG30">
         <v>2.25275360571686E-2</v>
       </c>
-      <c r="DG30">
+      <c r="DH30">
         <v>2.56178046984132E-2</v>
       </c>
-      <c r="DH30">
+      <c r="DI30">
         <v>-6.6810418211389298E-3</v>
       </c>
-      <c r="DI30">
+      <c r="DJ30">
         <f>CU30-CY30</f>
         <v>1.3752999948339895E-3</v>
       </c>
+      <c r="DK30">
+        <f>((CW30-CU30)/CU30)*100</f>
+        <v>3.2740629443776896</v>
+      </c>
     </row>
-    <row r="31" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
@@ -12217,32 +12433,39 @@
         <v>-8.5677397437393596E-3</v>
       </c>
       <c r="DB31" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC31">
+        <v>155</v>
+      </c>
+      <c r="DC31" t="s">
+        <v>207</v>
+      </c>
+      <c r="DD31">
         <v>-8.03946796804666E-3</v>
       </c>
-      <c r="DD31">
+      <c r="DE31">
         <v>-6.3296622829511701E-3</v>
       </c>
-      <c r="DE31">
+      <c r="DF31">
         <v>-2.1715800859965301E-2</v>
       </c>
-      <c r="DF31">
+      <c r="DG31">
         <v>-3.5533410264179102E-3</v>
       </c>
-      <c r="DG31">
+      <c r="DH31">
         <v>-1.8435353413224201E-3</v>
       </c>
-      <c r="DH31">
+      <c r="DI31">
         <v>1.5386138577014199E-2</v>
       </c>
-      <c r="DI31">
+      <c r="DJ31">
         <f>CU31-CY31</f>
         <v>-4.0404099272560168E-3</v>
       </c>
+      <c r="DK31">
+        <f>((CW31-CU31)/CU31)*100</f>
+        <v>3.4904434853992772</v>
+      </c>
     </row>
-    <row r="32" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -12577,32 +12800,39 @@
         <v>-9.1619975864887205E-4</v>
       </c>
       <c r="DB32" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC32">
+        <v>155</v>
+      </c>
+      <c r="DC32" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD32">
         <v>-1.49743710644543E-2</v>
       </c>
-      <c r="DD32">
+      <c r="DE32">
         <v>-0.111707811942324</v>
       </c>
-      <c r="DE32">
+      <c r="DF32">
         <v>-6.0706199845299097E-2</v>
       </c>
-      <c r="DF32">
+      <c r="DG32">
         <v>8.4945029113441706E-2</v>
       </c>
-      <c r="DG32">
+      <c r="DH32">
         <v>-1.1788411764428E-2</v>
       </c>
-      <c r="DH32">
+      <c r="DI32">
         <v>-5.1001612097024897E-2</v>
       </c>
-      <c r="DI32">
+      <c r="DJ32">
         <f>CU32-CY32</f>
         <v>2.1195899695158005E-2</v>
       </c>
+      <c r="DK32">
+        <f>((CW32-CU32)/CU32)*100</f>
+        <v>0.30674479103695773</v>
+      </c>
     </row>
-    <row r="33" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>15</v>
       </c>
@@ -12937,32 +13167,39 @@
         <v>4.36207861639559E-4</v>
       </c>
       <c r="DB33" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC33">
+        <v>155</v>
+      </c>
+      <c r="DC33" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD33">
         <v>-3.5793193412246099E-2</v>
       </c>
-      <c r="DD33">
+      <c r="DE33">
         <v>-6.5437516474048593E-2</v>
       </c>
-      <c r="DE33">
+      <c r="DF33">
         <v>-5.7254619503510101E-2</v>
       </c>
-      <c r="DF33">
+      <c r="DG33">
         <v>1.00231205287855E-2</v>
       </c>
-      <c r="DG33">
+      <c r="DH33">
         <v>-1.9621202533016899E-2</v>
       </c>
-      <c r="DH33">
+      <c r="DI33">
         <v>-8.1828969705384207E-3</v>
       </c>
-      <c r="DI33">
+      <c r="DJ33">
         <f>CU33-CY33</f>
         <v>-4.1779354796794843E-4</v>
       </c>
+      <c r="DK33">
+        <f>((CW33-CU33)/CU33)*100</f>
+        <v>-0.14043265374919442</v>
+      </c>
     </row>
-    <row r="34" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>58</v>
       </c>
@@ -13297,32 +13534,39 @@
         <v>1.46770582068711E-3</v>
       </c>
       <c r="DB34" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC34">
+        <v>155</v>
+      </c>
+      <c r="DC34" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD34">
         <v>-4.4672297779470599E-2</v>
       </c>
-      <c r="DD34">
+      <c r="DE34">
         <v>-4.11077875032788E-2</v>
       </c>
-      <c r="DE34">
+      <c r="DF34">
         <v>-9.9419740698067402E-2</v>
       </c>
-      <c r="DF34">
+      <c r="DG34">
         <v>-2.23971271334448E-2</v>
       </c>
-      <c r="DG34">
+      <c r="DH34">
         <v>-1.8832616857253001E-2</v>
       </c>
-      <c r="DH34">
+      <c r="DI34">
         <v>5.8311953194788602E-2</v>
       </c>
-      <c r="DI34">
+      <c r="DJ34">
         <f>CU34-CY34</f>
         <v>8.945549139752984E-3</v>
       </c>
+      <c r="DK34">
+        <f>((CW34-CU34)/CU34)*100</f>
+        <v>-0.47424801063530675</v>
+      </c>
     </row>
-    <row r="35" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
@@ -13657,32 +13901,39 @@
         <v>2.90569999197032E-3</v>
       </c>
       <c r="DB35" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC35">
+        <v>155</v>
+      </c>
+      <c r="DC35" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD35">
         <v>-6.0921791708096799E-2</v>
       </c>
-      <c r="DD35">
+      <c r="DE35">
         <v>-9.4863428967073508E-3</v>
       </c>
-      <c r="DE35">
+      <c r="DF35">
         <v>-3.01781923044472E-2</v>
       </c>
-      <c r="DF35">
+      <c r="DG35">
         <v>-4.1412376682274002E-2</v>
       </c>
-      <c r="DG35">
+      <c r="DH35">
         <v>1.00230721291154E-2</v>
       </c>
-      <c r="DH35">
+      <c r="DI35">
         <v>2.0691849407739899E-2</v>
       </c>
-      <c r="DI35">
+      <c r="DJ35">
         <f>CU35-CY35</f>
         <v>-7.1944000083020154E-3</v>
       </c>
+      <c r="DK35">
+        <f>((CW35-CU35)/CU35)*100</f>
+        <v>-0.90475997471162817</v>
+      </c>
     </row>
-    <row r="36" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -14017,32 +14268,39 @@
         <v>3.5974316997453501E-3</v>
       </c>
       <c r="DB36" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC36">
+        <v>155</v>
+      </c>
+      <c r="DC36" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD36">
         <v>3.12500000291038E-3</v>
       </c>
-      <c r="DD36">
+      <c r="DE36">
         <v>1.01001000002725E-2</v>
       </c>
-      <c r="DE36">
+      <c r="DF36">
         <v>2.1102499988046398E-2</v>
       </c>
-      <c r="DF36">
+      <c r="DG36">
         <v>-7.1944000083021802E-3</v>
       </c>
-      <c r="DG36">
+      <c r="DH36">
         <v>-2.1930001094005999E-4</v>
       </c>
-      <c r="DH36">
+      <c r="DI36">
         <v>-1.10023999877739E-2</v>
       </c>
-      <c r="DI36">
+      <c r="DJ36">
         <f>CU36-CY36</f>
         <v>-2.0272345282139614E-3</v>
       </c>
+      <c r="DK36">
+        <f>((CW36-CU36)/CU36)*100</f>
+        <v>-1.1719300994856181</v>
+      </c>
     </row>
-    <row r="37" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
@@ -14377,32 +14635,39 @@
         <v>3.8541569447261199E-3</v>
       </c>
       <c r="DB37" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC37">
+        <v>155</v>
+      </c>
+      <c r="DC37" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD37">
         <v>2.0173534401692401E-2</v>
       </c>
-      <c r="DD37">
+      <c r="DE37">
         <v>1.10234775056596E-2</v>
       </c>
-      <c r="DE37">
+      <c r="DF37">
         <v>-4.8836930654942903E-3</v>
       </c>
-      <c r="DF37">
+      <c r="DG37">
         <v>-6.1559346358990297E-3</v>
       </c>
-      <c r="DG37">
+      <c r="DH37">
         <v>-1.53059915319317E-2</v>
       </c>
-      <c r="DH37">
+      <c r="DI37">
         <v>1.59071705711539E-2</v>
       </c>
-      <c r="DI37">
+      <c r="DJ37">
         <f>CU37-CY37</f>
         <v>-1.9277576793690354E-3</v>
       </c>
+      <c r="DK37">
+        <f>((CW37-CU37)/CU37)*100</f>
+        <v>-1.2355858382006983</v>
+      </c>
     </row>
-    <row r="38" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
@@ -14737,32 +15002,39 @@
         <v>4.8675428697606497E-3</v>
       </c>
       <c r="DB38" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC38">
+        <v>155</v>
+      </c>
+      <c r="DC38" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD38">
         <v>-0.119005200045648</v>
       </c>
-      <c r="DD38">
+      <c r="DE38">
         <v>-9.4751600001472897E-2</v>
       </c>
-      <c r="DE38">
+      <c r="DF38">
         <v>-0.10928370000328801</v>
       </c>
-      <c r="DF38">
+      <c r="DG38">
         <v>-1.25930000212974E-2</v>
       </c>
-      <c r="DG38">
+      <c r="DH38">
         <v>1.1660600022878401E-2</v>
       </c>
-      <c r="DH38">
+      <c r="DI38">
         <v>1.45321000018157E-2</v>
       </c>
-      <c r="DI38">
+      <c r="DJ38">
         <f>CU38-CY38</f>
         <v>-6.1559346358989742E-3</v>
       </c>
+      <c r="DK38">
+        <f>((CW38-CU38)/CU38)*100</f>
+        <v>-1.4711390034728571</v>
+      </c>
     </row>
-    <row r="39" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>59</v>
       </c>
@@ -15097,32 +15369,39 @@
         <v>5.8379120018798797E-3</v>
       </c>
       <c r="DB39" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC39">
+        <v>155</v>
+      </c>
+      <c r="DC39" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD39">
         <v>-1.63951474823988E-2</v>
       </c>
-      <c r="DD39">
+      <c r="DE39">
         <v>-7.9860369442030701E-4</v>
       </c>
-      <c r="DE39">
+      <c r="DF39">
         <v>2.2472746204584799E-2</v>
       </c>
-      <c r="DF39">
+      <c r="DG39">
         <v>1.2935537844896299E-2</v>
       </c>
-      <c r="DG39">
+      <c r="DH39">
         <v>2.8532081632874899E-2</v>
       </c>
-      <c r="DH39">
+      <c r="DI39">
         <v>-2.32713498990051E-2</v>
       </c>
-      <c r="DI39">
+      <c r="DJ39">
         <f>CU39-CY39</f>
         <v>2.2527536057169006E-2</v>
       </c>
+      <c r="DK39">
+        <f>((CW39-CU39)/CU39)*100</f>
+        <v>-1.9346235549349606</v>
+      </c>
     </row>
-    <row r="40" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>52</v>
       </c>
@@ -15457,32 +15736,39 @@
         <v>6.2309500062838197E-3</v>
       </c>
       <c r="DB40" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC40">
+        <v>155</v>
+      </c>
+      <c r="DC40" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD40">
         <v>-1.3836700003594099E-2</v>
       </c>
-      <c r="DD40">
+      <c r="DE40">
         <v>-1.0015300002123599E-2</v>
       </c>
-      <c r="DE40">
+      <c r="DF40">
         <v>-1.5543000044999601E-3</v>
       </c>
-      <c r="DF40">
+      <c r="DG40">
         <v>1.37529999483376E-3</v>
       </c>
-      <c r="DG40">
+      <c r="DH40">
         <v>5.19669999630423E-3</v>
       </c>
-      <c r="DH40">
+      <c r="DI40">
         <v>-8.4609999976237305E-3</v>
       </c>
-      <c r="DI40">
+      <c r="DJ40">
         <f>CU40-CY40</f>
         <v>-1.543111767387001E-2</v>
       </c>
+      <c r="DK40">
+        <f>((CW40-CU40)/CU40)*100</f>
+        <v>-2.249879298736337</v>
+      </c>
     </row>
-    <row r="41" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>25</v>
       </c>
@@ -15817,32 +16103,39 @@
         <v>1.2136934150476E-2</v>
       </c>
       <c r="DB41" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC41">
+        <v>155</v>
+      </c>
+      <c r="DC41" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD41">
         <v>-0.11602759995730499</v>
       </c>
-      <c r="DD41">
+      <c r="DE41">
         <v>-7.9127300006803097E-2</v>
       </c>
-      <c r="DE41">
+      <c r="DF41">
         <v>1.23130999854765E-2</v>
       </c>
-      <c r="DF41">
+      <c r="DG41">
         <v>-6.7212299967650296E-2</v>
       </c>
-      <c r="DG41">
+      <c r="DH41">
         <v>-3.0312000017147501E-2</v>
       </c>
-      <c r="DH41">
+      <c r="DI41">
         <v>-9.1440399992279695E-2</v>
       </c>
-      <c r="DI41">
+      <c r="DJ41">
         <f>CU41-CY41</f>
         <v>1.2935537844896983E-2</v>
       </c>
+      <c r="DK41">
+        <f>((CW41-CU41)/CU41)*100</f>
+        <v>-4.0675381885920059</v>
+      </c>
     </row>
-    <row r="42" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
@@ -16177,32 +16470,39 @@
         <v>2.07562929717823E-2</v>
       </c>
       <c r="DB42" t="s">
-        <v>205</v>
-      </c>
-      <c r="DC42">
+        <v>155</v>
+      </c>
+      <c r="DC42" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD42">
         <v>-0.18023115000687501</v>
       </c>
-      <c r="DD42">
+      <c r="DE42">
         <v>-0.18237645016051801</v>
       </c>
-      <c r="DE42">
+      <c r="DF42">
         <v>-0.19274635007604901</v>
       </c>
-      <c r="DF42">
+      <c r="DG42">
         <v>-7.2201899951323797E-2</v>
       </c>
-      <c r="DG42">
+      <c r="DH42">
         <v>-7.4347200104966704E-2</v>
       </c>
-      <c r="DH42">
+      <c r="DI42">
         <v>1.03698999155312E-2</v>
       </c>
-      <c r="DI42">
+      <c r="DJ42">
         <f>CU42-CY42</f>
         <v>4.0549613069743029E-2</v>
       </c>
+      <c r="DK42">
+        <f>((CW42-CU42)/CU42)*100</f>
+        <v>-6.0429422073569805</v>
+      </c>
     </row>
-    <row r="43" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>36</v>
       </c>
@@ -16537,32 +16837,39 @@
         <v>3.5044225828187302E-2</v>
       </c>
       <c r="DB43" t="s">
-        <v>207</v>
-      </c>
-      <c r="DC43">
+        <v>155</v>
+      </c>
+      <c r="DC43" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD43">
         <v>-5.0415999721735699E-3</v>
       </c>
-      <c r="DD43">
+      <c r="DE43">
         <v>-2.5678499951027299E-2</v>
       </c>
-      <c r="DE43">
+      <c r="DF43">
         <v>-1.58514999784529E-2</v>
       </c>
-      <c r="DF43">
+      <c r="DG43">
         <v>1.0874099971260799E-2</v>
       </c>
-      <c r="DG43">
+      <c r="DH43">
         <v>-9.7628000075928797E-3</v>
       </c>
-      <c r="DH43">
+      <c r="DI43">
         <v>-9.8269999725744094E-3</v>
       </c>
-      <c r="DI43">
+      <c r="DJ43">
         <f>CU43-CY43</f>
         <v>3.1233236636579731E-3</v>
       </c>
+      <c r="DK43">
+        <f>((CW43-CU43)/CU43)*100</f>
+        <v>-11.071131059747085</v>
+      </c>
     </row>
-    <row r="44" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>21</v>
       </c>
@@ -16897,32 +17204,39 @@
         <v>5.40236873202957E-2</v>
       </c>
       <c r="DB44" t="s">
-        <v>207</v>
-      </c>
-      <c r="DC44">
+        <v>155</v>
+      </c>
+      <c r="DC44" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD44">
         <v>-8.8969799922779202E-2</v>
       </c>
-      <c r="DD44">
+      <c r="DE44">
         <v>-0.11786190001294</v>
       </c>
-      <c r="DE44">
+      <c r="DF44">
         <v>-5.7088499888777698E-2</v>
       </c>
-      <c r="DF44">
+      <c r="DG44">
         <v>-1.73576998058706E-2</v>
       </c>
-      <c r="DG44">
+      <c r="DH44">
         <v>-4.6249799896031597E-2</v>
       </c>
-      <c r="DH44">
+      <c r="DI44">
         <v>-6.0773400124162401E-2</v>
       </c>
-      <c r="DI44">
+      <c r="DJ44">
         <f>CU44-CY44</f>
         <v>6.8547371934983004E-2</v>
       </c>
+      <c r="DK44">
+        <f>((CW44-CU44)/CU44)*100</f>
+        <v>-14.324683868942911</v>
+      </c>
     </row>
-    <row r="45" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>41</v>
       </c>
@@ -17257,32 +17571,39 @@
         <v>6.4827359397895606E-2</v>
       </c>
       <c r="DB45" t="s">
-        <v>207</v>
-      </c>
-      <c r="DC45">
+        <v>155</v>
+      </c>
+      <c r="DC45" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD45">
         <v>-1.5547099988907499E-2</v>
       </c>
-      <c r="DD45">
+      <c r="DE45">
         <v>-4.81179000344127E-2</v>
       </c>
-      <c r="DE45">
+      <c r="DF45">
         <v>5.6025799945928101E-2</v>
       </c>
-      <c r="DF45">
+      <c r="DG45">
         <v>-3.0303999083116599E-3</v>
       </c>
-      <c r="DG45">
+      <c r="DH45">
         <v>-3.5601199953816803E-2</v>
       </c>
-      <c r="DH45">
+      <c r="DI45">
         <v>-0.10414369998034</v>
       </c>
-      <c r="DI45">
+      <c r="DJ45">
         <f>CU45-CY45</f>
         <v>1.1723811156117037E-2</v>
       </c>
+      <c r="DK45">
+        <f>((CW45-CU45)/CU45)*100</f>
+        <v>-19.384938430286315</v>
+      </c>
     </row>
-    <row r="46" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -17617,32 +17938,39 @@
         <v>7.3251906142104403E-2</v>
       </c>
       <c r="DB46" t="s">
-        <v>207</v>
-      </c>
-      <c r="DC46">
+        <v>155</v>
+      </c>
+      <c r="DC46" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD46">
         <v>-2.7425399515777799E-2</v>
       </c>
-      <c r="DD46">
+      <c r="DE46">
         <v>-2.2112099453806801E-2</v>
       </c>
-      <c r="DE46">
+      <c r="DF46">
         <v>2.7295006439089701E-3</v>
       </c>
-      <c r="DF46">
+      <c r="DG46">
         <v>2.1195899695158001E-2</v>
       </c>
-      <c r="DG46">
+      <c r="DH46">
         <v>2.6509199757128898E-2</v>
       </c>
-      <c r="DH46">
+      <c r="DI46">
         <v>-2.4841600097715799E-2</v>
       </c>
-      <c r="DI46">
+      <c r="DJ46">
         <f>CU46-CY46</f>
         <v>8.0505915102548953E-2</v>
       </c>
+      <c r="DK46">
+        <f>((CW46-CU46)/CU46)*100</f>
+        <v>-13.098325160143276</v>
+      </c>
     </row>
-    <row r="47" spans="1:113" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:115" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -17977,33 +18305,40 @@
         <v>7.6968276669504093E-2</v>
       </c>
       <c r="DB47" t="s">
-        <v>207</v>
-      </c>
-      <c r="DC47">
+        <v>155</v>
+      </c>
+      <c r="DC47" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD47">
         <v>7.7434499748051097E-2</v>
       </c>
-      <c r="DD47">
+      <c r="DE47">
         <v>-2.6286300038918801E-2</v>
       </c>
-      <c r="DE47">
+      <c r="DF47">
         <v>7.5395000167191001E-2</v>
       </c>
-      <c r="DF47">
+      <c r="DG47">
         <v>6.3898500520735901E-3</v>
       </c>
-      <c r="DG47">
+      <c r="DH47">
         <v>-9.7330949734896394E-2</v>
       </c>
-      <c r="DH47">
+      <c r="DI47">
         <v>-0.10168130020610899</v>
       </c>
-      <c r="DI47">
+      <c r="DJ47">
         <f>CU47-CY47</f>
         <v>4.2992998933186977E-2</v>
       </c>
+      <c r="DK47">
+        <f>((CW47-CU47)/CU47)*100</f>
+        <v>-25.920296920629426</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DI47">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DK47">
     <sortCondition ref="DA1:DA47"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
add sztats for SG & SL
</commit_message>
<xml_diff>
--- a/code/total_df_n46.xlsx
+++ b/code/total_df_n46.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-mid-clean/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB61A77-8FA7-1B4C-92AF-3DAF5CE3B6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FCBFA0-2CB0-8D44-96FA-A2604FE06D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1220" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1099,7 +1099,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="BM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BW49" sqref="BW49:BX49"/>
+      <selection pane="bottomRight" activeCell="BU1" sqref="BU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>